<commit_message>
merge latest survey data 2023_11
</commit_message>
<xml_diff>
--- a/data/survey_data.xlsx
+++ b/data/survey_data.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/cgarcia/Documents/IHCC/Atlas/Excel surveys to upload to Github/Update November 2023/Survey file - to upload/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{41A74E15-9C99-A643-A74C-DC4479B71B67}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B4BC9921-9470-3D4D-921E-530CB31211BC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="38400" windowHeight="19700" tabRatio="500" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -110,7 +110,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2679" uniqueCount="535">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2736" uniqueCount="532">
   <si>
     <t>IHCC Data Harmonization</t>
   </si>
@@ -1259,9 +1259,6 @@
     <t>Population-based, random sample</t>
   </si>
   <si>
-    <t>100% of cohort</t>
-  </si>
-  <si>
     <t>76-100% of cohort</t>
     <phoneticPr fontId="0"/>
   </si>
@@ -1321,9 +1318,6 @@
   </si>
   <si>
     <t>Y - 26-50% of cohort</t>
-  </si>
-  <si>
-    <t>% Uknown</t>
   </si>
   <si>
     <t>Southeastern Asia</t>
@@ -1753,9 +1747,6 @@
   </si>
   <si>
     <t>Yes - 51-75% of cohort</t>
-  </si>
-  <si>
-    <t>Yes - 100% of cohort</t>
   </si>
   <si>
     <t>Y - Yes - 76-100% of cohort</t>
@@ -2906,9 +2897,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:CJ48"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="117" zoomScaleNormal="117" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A2" zoomScale="114" zoomScaleNormal="114" workbookViewId="0">
       <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="BW13" sqref="BW13"/>
+      <selection pane="topRight" activeCell="M48" sqref="M48"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="27.6640625" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
@@ -2927,265 +2918,265 @@
         <v>5</v>
       </c>
       <c r="B2" s="58" t="s">
+        <v>409</v>
+      </c>
+      <c r="C2" s="58" t="s">
+        <v>410</v>
+      </c>
+      <c r="D2" s="58" t="s">
         <v>411</v>
       </c>
-      <c r="C2" s="58" t="s">
+      <c r="E2" s="58" t="s">
         <v>412</v>
       </c>
-      <c r="D2" s="58" t="s">
+      <c r="F2" s="58" t="s">
         <v>413</v>
       </c>
-      <c r="E2" s="58" t="s">
+      <c r="G2" s="58" t="s">
         <v>414</v>
       </c>
-      <c r="F2" s="58" t="s">
+      <c r="H2" s="58" t="s">
         <v>415</v>
       </c>
-      <c r="G2" s="58" t="s">
+      <c r="I2" s="58" t="s">
         <v>416</v>
       </c>
-      <c r="H2" s="58" t="s">
+      <c r="J2" s="58" t="s">
         <v>417</v>
       </c>
-      <c r="I2" s="58" t="s">
+      <c r="K2" s="58" t="s">
         <v>418</v>
       </c>
-      <c r="J2" s="58" t="s">
+      <c r="L2" s="58" t="s">
         <v>419</v>
       </c>
-      <c r="K2" s="58" t="s">
+      <c r="M2" s="58" t="s">
         <v>420</v>
       </c>
-      <c r="L2" s="58" t="s">
+      <c r="N2" s="58" t="s">
         <v>421</v>
       </c>
-      <c r="M2" s="58" t="s">
+      <c r="O2" s="58" t="s">
         <v>422</v>
       </c>
-      <c r="N2" s="58" t="s">
+      <c r="P2" s="58" t="s">
         <v>423</v>
       </c>
-      <c r="O2" s="58" t="s">
+      <c r="Q2" s="58" t="s">
         <v>424</v>
       </c>
-      <c r="P2" s="58" t="s">
+      <c r="R2" s="58" t="s">
         <v>425</v>
       </c>
-      <c r="Q2" s="58" t="s">
+      <c r="S2" s="58" t="s">
         <v>426</v>
       </c>
-      <c r="R2" s="58" t="s">
+      <c r="T2" s="58" t="s">
         <v>427</v>
       </c>
-      <c r="S2" s="58" t="s">
+      <c r="U2" s="58" t="s">
         <v>428</v>
       </c>
-      <c r="T2" s="58" t="s">
+      <c r="V2" s="58" t="s">
         <v>429</v>
       </c>
-      <c r="U2" s="58" t="s">
+      <c r="W2" s="58" t="s">
         <v>430</v>
       </c>
-      <c r="V2" s="58" t="s">
+      <c r="X2" s="58" t="s">
         <v>431</v>
       </c>
-      <c r="W2" s="58" t="s">
+      <c r="Y2" s="58" t="s">
         <v>432</v>
       </c>
-      <c r="X2" s="58" t="s">
+      <c r="Z2" s="58" t="s">
         <v>433</v>
       </c>
-      <c r="Y2" s="58" t="s">
+      <c r="AA2" s="58" t="s">
         <v>434</v>
       </c>
-      <c r="Z2" s="58" t="s">
+      <c r="AB2" s="58" t="s">
         <v>435</v>
       </c>
-      <c r="AA2" s="58" t="s">
+      <c r="AC2" s="58" t="s">
         <v>436</v>
       </c>
-      <c r="AB2" s="58" t="s">
+      <c r="AD2" s="58" t="s">
         <v>437</v>
       </c>
-      <c r="AC2" s="58" t="s">
+      <c r="AE2" s="58" t="s">
         <v>438</v>
       </c>
-      <c r="AD2" s="58" t="s">
+      <c r="AF2" s="58" t="s">
         <v>439</v>
       </c>
-      <c r="AE2" s="58" t="s">
+      <c r="AG2" s="58" t="s">
         <v>440</v>
       </c>
-      <c r="AF2" s="58" t="s">
+      <c r="AH2" s="58" t="s">
         <v>441</v>
       </c>
-      <c r="AG2" s="58" t="s">
+      <c r="AI2" s="58" t="s">
         <v>442</v>
       </c>
-      <c r="AH2" s="58" t="s">
+      <c r="AJ2" s="58" t="s">
         <v>443</v>
       </c>
-      <c r="AI2" s="58" t="s">
+      <c r="AK2" s="58" t="s">
         <v>444</v>
       </c>
-      <c r="AJ2" s="58" t="s">
+      <c r="AL2" s="58" t="s">
         <v>445</v>
       </c>
-      <c r="AK2" s="58" t="s">
+      <c r="AM2" s="58" t="s">
         <v>446</v>
       </c>
-      <c r="AL2" s="58" t="s">
+      <c r="AN2" s="58" t="s">
         <v>447</v>
       </c>
-      <c r="AM2" s="58" t="s">
+      <c r="AO2" s="58" t="s">
         <v>448</v>
       </c>
-      <c r="AN2" s="58" t="s">
+      <c r="AP2" s="58" t="s">
         <v>449</v>
-      </c>
-      <c r="AO2" s="58" t="s">
-        <v>450</v>
-      </c>
-      <c r="AP2" s="58" t="s">
-        <v>451</v>
       </c>
       <c r="AQ2" s="58" t="s">
         <v>313</v>
       </c>
       <c r="AR2" s="58" t="s">
+        <v>450</v>
+      </c>
+      <c r="AS2" s="58" t="s">
+        <v>451</v>
+      </c>
+      <c r="AT2" s="58" t="s">
         <v>452</v>
       </c>
-      <c r="AS2" s="58" t="s">
+      <c r="AU2" s="58" t="s">
         <v>453</v>
       </c>
-      <c r="AT2" s="58" t="s">
+      <c r="AV2" s="58" t="s">
         <v>454</v>
       </c>
-      <c r="AU2" s="58" t="s">
+      <c r="AW2" s="58" t="s">
         <v>455</v>
       </c>
-      <c r="AV2" s="58" t="s">
+      <c r="AX2" s="58" t="s">
+        <v>494</v>
+      </c>
+      <c r="AY2" s="58" t="s">
         <v>456</v>
       </c>
-      <c r="AW2" s="58" t="s">
+      <c r="AZ2" s="58" t="s">
         <v>457</v>
       </c>
-      <c r="AX2" s="58" t="s">
-        <v>496</v>
-      </c>
-      <c r="AY2" s="58" t="s">
+      <c r="BA2" s="58" t="s">
         <v>458</v>
       </c>
-      <c r="AZ2" s="58" t="s">
+      <c r="BB2" s="58" t="s">
         <v>459</v>
       </c>
-      <c r="BA2" s="58" t="s">
+      <c r="BC2" s="58" t="s">
         <v>460</v>
       </c>
-      <c r="BB2" s="58" t="s">
+      <c r="BD2" s="58" t="s">
         <v>461</v>
       </c>
-      <c r="BC2" s="58" t="s">
+      <c r="BE2" s="58" t="s">
         <v>462</v>
       </c>
-      <c r="BD2" s="58" t="s">
+      <c r="BF2" s="58" t="s">
         <v>463</v>
       </c>
-      <c r="BE2" s="58" t="s">
+      <c r="BG2" s="58" t="s">
         <v>464</v>
       </c>
-      <c r="BF2" s="58" t="s">
+      <c r="BH2" s="58" t="s">
         <v>465</v>
       </c>
-      <c r="BG2" s="58" t="s">
+      <c r="BI2" s="58" t="s">
         <v>466</v>
       </c>
-      <c r="BH2" s="58" t="s">
+      <c r="BJ2" s="58" t="s">
         <v>467</v>
       </c>
-      <c r="BI2" s="58" t="s">
+      <c r="BK2" s="58" t="s">
         <v>468</v>
       </c>
-      <c r="BJ2" s="58" t="s">
+      <c r="BL2" s="58" t="s">
         <v>469</v>
       </c>
-      <c r="BK2" s="58" t="s">
+      <c r="BM2" s="58" t="s">
         <v>470</v>
       </c>
-      <c r="BL2" s="58" t="s">
+      <c r="BN2" s="58" t="s">
         <v>471</v>
       </c>
-      <c r="BM2" s="58" t="s">
+      <c r="BO2" s="58" t="s">
         <v>472</v>
       </c>
-      <c r="BN2" s="58" t="s">
+      <c r="BP2" s="58" t="s">
         <v>473</v>
       </c>
-      <c r="BO2" s="58" t="s">
+      <c r="BQ2" s="58" t="s">
         <v>474</v>
       </c>
-      <c r="BP2" s="58" t="s">
+      <c r="BR2" s="58" t="s">
         <v>475</v>
       </c>
-      <c r="BQ2" s="58" t="s">
+      <c r="BS2" s="58" t="s">
         <v>476</v>
       </c>
-      <c r="BR2" s="58" t="s">
+      <c r="BT2" s="58" t="s">
         <v>477</v>
       </c>
-      <c r="BS2" s="58" t="s">
+      <c r="BU2" s="58" t="s">
         <v>478</v>
       </c>
-      <c r="BT2" s="58" t="s">
+      <c r="BV2" s="58" t="s">
         <v>479</v>
       </c>
-      <c r="BU2" s="58" t="s">
+      <c r="BW2" s="58" t="s">
         <v>480</v>
       </c>
-      <c r="BV2" s="58" t="s">
+      <c r="BX2" s="58" t="s">
         <v>481</v>
       </c>
-      <c r="BW2" s="58" t="s">
+      <c r="BY2" s="58" t="s">
         <v>482</v>
       </c>
-      <c r="BX2" s="58" t="s">
+      <c r="BZ2" s="58" t="s">
         <v>483</v>
       </c>
-      <c r="BY2" s="58" t="s">
+      <c r="CA2" s="58" t="s">
         <v>484</v>
       </c>
-      <c r="BZ2" s="58" t="s">
+      <c r="CB2" s="58" t="s">
         <v>485</v>
       </c>
-      <c r="CA2" s="58" t="s">
+      <c r="CC2" s="58" t="s">
         <v>486</v>
       </c>
-      <c r="CB2" s="58" t="s">
+      <c r="CD2" s="58" t="s">
         <v>487</v>
       </c>
-      <c r="CC2" s="58" t="s">
+      <c r="CE2" s="58" t="s">
         <v>488</v>
       </c>
-      <c r="CD2" s="58" t="s">
+      <c r="CF2" s="58" t="s">
         <v>489</v>
       </c>
-      <c r="CE2" s="58" t="s">
+      <c r="CG2" s="58" t="s">
         <v>490</v>
       </c>
-      <c r="CF2" s="58" t="s">
+      <c r="CH2" s="58" t="s">
         <v>491</v>
       </c>
-      <c r="CG2" s="58" t="s">
+      <c r="CI2" s="58" t="s">
         <v>492</v>
       </c>
-      <c r="CH2" s="58" t="s">
+      <c r="CJ2" s="58" t="s">
         <v>493</v>
-      </c>
-      <c r="CI2" s="58" t="s">
-        <v>494</v>
-      </c>
-      <c r="CJ2" s="58" t="s">
-        <v>495</v>
       </c>
     </row>
     <row r="3" spans="1:88" s="15" customFormat="1" ht="57" x14ac:dyDescent="0.2">
@@ -3196,22 +3187,22 @@
         <v>47</v>
       </c>
       <c r="C3" s="86" t="s">
-        <v>497</v>
+        <v>495</v>
       </c>
       <c r="D3" s="86" t="s">
         <v>64</v>
       </c>
       <c r="E3" s="58" t="s">
-        <v>498</v>
+        <v>496</v>
       </c>
       <c r="F3" s="87" t="s">
         <v>285</v>
       </c>
       <c r="G3" s="58" t="s">
-        <v>522</v>
+        <v>520</v>
       </c>
       <c r="H3" s="58" t="s">
-        <v>499</v>
+        <v>497</v>
       </c>
       <c r="I3" s="88" t="s">
         <v>288</v>
@@ -3220,28 +3211,28 @@
         <v>289</v>
       </c>
       <c r="K3" s="58" t="s">
-        <v>500</v>
+        <v>498</v>
       </c>
       <c r="L3" s="88" t="s">
         <v>291</v>
       </c>
       <c r="M3" s="58" t="s">
-        <v>501</v>
+        <v>499</v>
       </c>
       <c r="N3" s="58" t="s">
-        <v>502</v>
+        <v>500</v>
       </c>
       <c r="O3" s="58" t="s">
         <v>52</v>
       </c>
       <c r="P3" s="58" t="s">
+        <v>501</v>
+      </c>
+      <c r="Q3" s="58" t="s">
+        <v>502</v>
+      </c>
+      <c r="R3" s="58" t="s">
         <v>503</v>
-      </c>
-      <c r="Q3" s="58" t="s">
-        <v>504</v>
-      </c>
-      <c r="R3" s="58" t="s">
-        <v>505</v>
       </c>
       <c r="S3" s="58" t="s">
         <v>57</v>
@@ -3256,7 +3247,7 @@
         <v>297</v>
       </c>
       <c r="W3" s="58" t="s">
-        <v>506</v>
+        <v>504</v>
       </c>
       <c r="X3" s="87" t="s">
         <v>299</v>
@@ -3277,7 +3268,7 @@
         <v>43</v>
       </c>
       <c r="AD3" s="58" t="s">
-        <v>507</v>
+        <v>505</v>
       </c>
       <c r="AE3" s="90" t="s">
         <v>302</v>
@@ -3286,19 +3277,19 @@
         <v>303</v>
       </c>
       <c r="AG3" s="58" t="s">
-        <v>404</v>
+        <v>402</v>
       </c>
       <c r="AH3" s="58" t="s">
-        <v>509</v>
+        <v>507</v>
       </c>
       <c r="AI3" s="42" t="s">
-        <v>510</v>
+        <v>508</v>
       </c>
       <c r="AJ3" s="58" t="s">
         <v>59</v>
       </c>
       <c r="AK3" s="58" t="s">
-        <v>511</v>
+        <v>509</v>
       </c>
       <c r="AL3" s="88" t="s">
         <v>308</v>
@@ -3307,13 +3298,13 @@
         <v>56</v>
       </c>
       <c r="AN3" s="58" t="s">
-        <v>512</v>
+        <v>510</v>
       </c>
       <c r="AO3" s="58" t="s">
         <v>46</v>
       </c>
       <c r="AP3" s="58" t="s">
-        <v>513</v>
+        <v>511</v>
       </c>
       <c r="AQ3" s="90" t="s">
         <v>313</v>
@@ -3322,7 +3313,7 @@
         <v>63</v>
       </c>
       <c r="AS3" s="42" t="s">
-        <v>514</v>
+        <v>512</v>
       </c>
       <c r="AT3" s="58" t="s">
         <v>315</v>
@@ -3331,19 +3322,19 @@
         <v>218</v>
       </c>
       <c r="AV3" s="42" t="s">
-        <v>516</v>
+        <v>514</v>
       </c>
       <c r="AW3" s="58" t="s">
-        <v>517</v>
+        <v>515</v>
       </c>
       <c r="AX3" s="90" t="s">
         <v>321</v>
       </c>
       <c r="AY3" s="58" t="s">
-        <v>518</v>
+        <v>516</v>
       </c>
       <c r="AZ3" s="58" t="s">
-        <v>519</v>
+        <v>517</v>
       </c>
       <c r="BA3" s="42" t="s">
         <v>44</v>
@@ -3367,7 +3358,7 @@
         <v>51</v>
       </c>
       <c r="BH3" s="58" t="s">
-        <v>520</v>
+        <v>518</v>
       </c>
       <c r="BI3" s="58" t="s">
         <v>54</v>
@@ -3394,7 +3385,7 @@
         <v>49</v>
       </c>
       <c r="BQ3" s="42" t="s">
-        <v>521</v>
+        <v>519</v>
       </c>
       <c r="BR3" s="63" t="s">
         <v>50</v>
@@ -3972,25 +3963,25 @@
         <v>105</v>
       </c>
       <c r="F10" s="40" t="s">
+        <v>370</v>
+      </c>
+      <c r="G10" s="40" t="s">
         <v>371</v>
       </c>
-      <c r="G10" s="40" t="s">
+      <c r="H10" s="40" t="s">
+        <v>406</v>
+      </c>
+      <c r="I10" s="40" t="s">
         <v>372</v>
       </c>
-      <c r="H10" s="40" t="s">
-        <v>408</v>
-      </c>
-      <c r="I10" s="40" t="s">
+      <c r="J10" s="40" t="s">
         <v>373</v>
       </c>
-      <c r="J10" s="40" t="s">
+      <c r="K10" s="40" t="s">
         <v>374</v>
       </c>
-      <c r="K10" s="40" t="s">
+      <c r="L10" s="40" t="s">
         <v>375</v>
-      </c>
-      <c r="L10" s="40" t="s">
-        <v>376</v>
       </c>
       <c r="M10" s="40" t="s">
         <v>199</v>
@@ -4013,17 +4004,17 @@
         <v>100</v>
       </c>
       <c r="U10" s="40" t="s">
+        <v>376</v>
+      </c>
+      <c r="V10" s="40" t="s">
         <v>377</v>
-      </c>
-      <c r="V10" s="40" t="s">
-        <v>378</v>
       </c>
       <c r="W10" s="40" t="s">
         <v>80</v>
       </c>
       <c r="X10" s="40"/>
       <c r="Y10" s="40" t="s">
-        <v>379</v>
+        <v>378</v>
       </c>
       <c r="Z10" s="40" t="s">
         <v>82</v>
@@ -4046,7 +4037,7 @@
         <v>95</v>
       </c>
       <c r="AH10" s="79" t="s">
-        <v>406</v>
+        <v>404</v>
       </c>
       <c r="AI10" s="40" t="s">
         <v>97</v>
@@ -4056,16 +4047,16 @@
         <v>230</v>
       </c>
       <c r="AL10" s="40" t="s">
+        <v>379</v>
+      </c>
+      <c r="AM10" s="40" t="s">
         <v>380</v>
-      </c>
-      <c r="AM10" s="40" t="s">
-        <v>381</v>
       </c>
       <c r="AN10" s="40" t="s">
         <v>92</v>
       </c>
       <c r="AO10" s="40" t="s">
-        <v>382</v>
+        <v>381</v>
       </c>
       <c r="AP10" s="40" t="s">
         <v>103</v>
@@ -4090,7 +4081,7 @@
         <v>90</v>
       </c>
       <c r="AX10" s="82" t="s">
-        <v>384</v>
+        <v>383</v>
       </c>
       <c r="AY10" s="81" t="s">
         <v>274</v>
@@ -4103,14 +4094,14 @@
         <v>101</v>
       </c>
       <c r="BC10" s="81" t="s">
-        <v>383</v>
+        <v>382</v>
       </c>
       <c r="BD10" s="82" t="s">
         <v>96</v>
       </c>
       <c r="BE10" s="40"/>
       <c r="BF10" s="40" t="s">
-        <v>385</v>
+        <v>384</v>
       </c>
       <c r="BG10" s="40" t="s">
         <v>88</v>
@@ -4126,13 +4117,13 @@
       </c>
       <c r="BK10" s="58"/>
       <c r="BL10" s="40" t="s">
-        <v>386</v>
+        <v>385</v>
       </c>
       <c r="BM10" s="40" t="s">
         <v>237</v>
       </c>
       <c r="BN10" s="40" t="s">
-        <v>387</v>
+        <v>386</v>
       </c>
       <c r="BO10" s="58"/>
       <c r="BP10" s="40" t="s">
@@ -4184,7 +4175,7 @@
         <v>279</v>
       </c>
       <c r="CF10" s="26" t="s">
-        <v>407</v>
+        <v>405</v>
       </c>
       <c r="CG10" s="26" t="s">
         <v>236</v>
@@ -4486,7 +4477,7 @@
         <v>145</v>
       </c>
       <c r="H12" s="68" t="s">
-        <v>391</v>
+        <v>389</v>
       </c>
       <c r="I12" s="68" t="s">
         <v>359</v>
@@ -4528,7 +4519,7 @@
         <v>159</v>
       </c>
       <c r="V12" s="68" t="s">
-        <v>392</v>
+        <v>390</v>
       </c>
       <c r="W12" s="69" t="s">
         <v>143</v>
@@ -4540,7 +4531,7 @@
         <v>256</v>
       </c>
       <c r="Z12" s="70" t="s">
-        <v>393</v>
+        <v>391</v>
       </c>
       <c r="AA12" s="68" t="s">
         <v>150</v>
@@ -4633,10 +4624,10 @@
         <v>151</v>
       </c>
       <c r="BE12" s="68" t="s">
-        <v>394</v>
+        <v>392</v>
       </c>
       <c r="BF12" s="71" t="s">
-        <v>390</v>
+        <v>388</v>
       </c>
       <c r="BG12" s="69" t="s">
         <v>149</v>
@@ -4734,34 +4725,34 @@
         <v>23</v>
       </c>
       <c r="B13" s="58" t="s">
-        <v>531</v>
+        <v>529</v>
       </c>
       <c r="C13" s="58" t="s">
         <v>162</v>
       </c>
       <c r="D13" s="3" t="s">
-        <v>533</v>
+        <v>162</v>
       </c>
       <c r="E13" s="3" t="s">
-        <v>533</v>
+        <v>162</v>
       </c>
       <c r="H13" s="3" t="s">
-        <v>533</v>
+        <v>162</v>
       </c>
       <c r="J13" s="58" t="s">
-        <v>388</v>
+        <v>387</v>
       </c>
       <c r="M13" s="3" t="s">
-        <v>533</v>
+        <v>162</v>
       </c>
       <c r="N13" t="s">
-        <v>534</v>
+        <v>531</v>
       </c>
       <c r="O13" t="s">
-        <v>534</v>
+        <v>531</v>
       </c>
       <c r="P13" s="3" t="s">
-        <v>533</v>
+        <v>162</v>
       </c>
       <c r="Q13" s="58" t="s">
         <v>162</v>
@@ -4776,10 +4767,10 @@
         <v>162</v>
       </c>
       <c r="V13" s="3" t="s">
-        <v>533</v>
+        <v>162</v>
       </c>
       <c r="W13" s="3" t="s">
-        <v>533</v>
+        <v>162</v>
       </c>
       <c r="Z13" s="58" t="s">
         <v>162</v>
@@ -4791,73 +4782,73 @@
         <v>162</v>
       </c>
       <c r="AC13" s="3" t="s">
-        <v>533</v>
+        <v>162</v>
       </c>
       <c r="AE13" s="3" t="s">
-        <v>533</v>
+        <v>162</v>
       </c>
       <c r="AF13" t="s">
         <v>163</v>
       </c>
       <c r="AG13" s="3" t="s">
-        <v>533</v>
+        <v>162</v>
       </c>
       <c r="AH13" s="3" t="s">
-        <v>533</v>
+        <v>162</v>
       </c>
       <c r="AI13" s="3" t="s">
-        <v>533</v>
+        <v>162</v>
       </c>
       <c r="AJ13" s="58" t="s">
-        <v>531</v>
+        <v>529</v>
       </c>
       <c r="AK13" s="3" t="s">
-        <v>533</v>
+        <v>162</v>
       </c>
       <c r="AL13" s="3" t="s">
-        <v>533</v>
+        <v>162</v>
       </c>
       <c r="AM13" s="3" t="s">
-        <v>533</v>
+        <v>162</v>
       </c>
       <c r="AN13" s="58" t="s">
         <v>162</v>
       </c>
       <c r="AO13" s="3" t="s">
-        <v>533</v>
+        <v>162</v>
       </c>
       <c r="AP13" s="58" t="s">
         <v>162</v>
       </c>
       <c r="AR13" s="58" t="s">
-        <v>530</v>
+        <v>528</v>
       </c>
       <c r="AS13" t="s">
         <v>282</v>
       </c>
       <c r="AT13" s="3" t="s">
-        <v>533</v>
+        <v>162</v>
       </c>
       <c r="AU13" s="3" t="s">
-        <v>533</v>
+        <v>162</v>
       </c>
       <c r="AV13" s="3" t="s">
-        <v>533</v>
+        <v>162</v>
       </c>
       <c r="AW13" s="58" t="s">
         <v>162</v>
       </c>
       <c r="AX13" s="3" t="s">
-        <v>533</v>
+        <v>162</v>
       </c>
       <c r="AY13" s="3" t="s">
-        <v>533</v>
+        <v>162</v>
       </c>
       <c r="AZ13" t="s">
         <v>163</v>
       </c>
       <c r="BA13" s="3" t="s">
-        <v>533</v>
+        <v>162</v>
       </c>
       <c r="BB13" s="58" t="s">
         <v>162</v>
@@ -4878,7 +4869,7 @@
         <v>163</v>
       </c>
       <c r="BH13" s="3" t="s">
-        <v>533</v>
+        <v>162</v>
       </c>
       <c r="BI13" t="s">
         <v>163</v>
@@ -4893,7 +4884,7 @@
         <v>162</v>
       </c>
       <c r="BM13" s="3" t="s">
-        <v>533</v>
+        <v>162</v>
       </c>
       <c r="BN13" s="58" t="s">
         <v>162</v>
@@ -5842,6 +5833,9 @@
       <c r="N18" t="s">
         <v>74</v>
       </c>
+      <c r="O18" s="42" t="s">
+        <v>75</v>
+      </c>
       <c r="P18" t="s">
         <v>74</v>
       </c>
@@ -6066,13 +6060,60 @@
       <c r="A19" s="3" t="s">
         <v>72</v>
       </c>
-      <c r="B19" s="42"/>
-      <c r="D19" s="42"/>
-      <c r="H19" s="42"/>
-      <c r="I19" s="42"/>
-      <c r="J19" s="42"/>
-      <c r="L19" s="42"/>
-      <c r="R19" s="42"/>
+      <c r="B19" s="42" t="s">
+        <v>75</v>
+      </c>
+      <c r="C19" s="42" t="s">
+        <v>75</v>
+      </c>
+      <c r="D19" s="42" t="s">
+        <v>75</v>
+      </c>
+      <c r="E19" s="42" t="s">
+        <v>75</v>
+      </c>
+      <c r="F19" s="42" t="s">
+        <v>75</v>
+      </c>
+      <c r="G19" s="42" t="s">
+        <v>75</v>
+      </c>
+      <c r="H19" s="42" t="s">
+        <v>75</v>
+      </c>
+      <c r="I19" s="42" t="s">
+        <v>75</v>
+      </c>
+      <c r="J19" s="42" t="s">
+        <v>75</v>
+      </c>
+      <c r="K19" s="42" t="s">
+        <v>75</v>
+      </c>
+      <c r="L19" s="42" t="s">
+        <v>75</v>
+      </c>
+      <c r="M19" s="42" t="s">
+        <v>75</v>
+      </c>
+      <c r="N19" s="42" t="s">
+        <v>75</v>
+      </c>
+      <c r="O19" s="42" t="s">
+        <v>75</v>
+      </c>
+      <c r="P19" s="42" t="s">
+        <v>75</v>
+      </c>
+      <c r="Q19" s="42" t="s">
+        <v>75</v>
+      </c>
+      <c r="R19" s="42" t="s">
+        <v>75</v>
+      </c>
+      <c r="S19" s="42" t="s">
+        <v>75</v>
+      </c>
       <c r="T19" s="42" t="s">
         <v>75</v>
       </c>
@@ -6103,31 +6144,126 @@
       <c r="AC19" t="s">
         <v>365</v>
       </c>
+      <c r="AD19" s="42" t="s">
+        <v>75</v>
+      </c>
       <c r="AE19" t="s">
         <v>366</v>
       </c>
-      <c r="AF19" s="42"/>
-      <c r="AI19" s="42"/>
-      <c r="AK19" s="42"/>
-      <c r="AL19" s="42"/>
+      <c r="AF19" s="42" t="s">
+        <v>75</v>
+      </c>
+      <c r="AG19" s="42" t="s">
+        <v>75</v>
+      </c>
+      <c r="AH19" s="42" t="s">
+        <v>75</v>
+      </c>
+      <c r="AI19" s="42" t="s">
+        <v>75</v>
+      </c>
+      <c r="AJ19" s="42" t="s">
+        <v>75</v>
+      </c>
+      <c r="AK19" s="42" t="s">
+        <v>75</v>
+      </c>
+      <c r="AL19" s="42" t="s">
+        <v>75</v>
+      </c>
+      <c r="AM19" s="42" t="s">
+        <v>75</v>
+      </c>
       <c r="AN19" t="s">
         <v>367</v>
       </c>
-      <c r="AO19" s="42"/>
-      <c r="AR19" s="42"/>
-      <c r="AS19" s="42"/>
-      <c r="AV19" s="42"/>
-      <c r="AX19" s="42"/>
-      <c r="AZ19" s="42"/>
-      <c r="BA19" s="42"/>
-      <c r="BB19" s="42"/>
-      <c r="BC19" s="42"/>
-      <c r="BE19" s="42"/>
-      <c r="BJ19" s="42"/>
-      <c r="BK19" s="42"/>
-      <c r="BL19" s="42"/>
-      <c r="BN19" s="42"/>
-      <c r="BQ19" s="42"/>
+      <c r="AO19" s="42" t="s">
+        <v>75</v>
+      </c>
+      <c r="AP19" s="42" t="s">
+        <v>75</v>
+      </c>
+      <c r="AQ19" s="42" t="s">
+        <v>75</v>
+      </c>
+      <c r="AR19" s="42" t="s">
+        <v>75</v>
+      </c>
+      <c r="AS19" s="42" t="s">
+        <v>75</v>
+      </c>
+      <c r="AT19" s="42" t="s">
+        <v>75</v>
+      </c>
+      <c r="AU19" s="42" t="s">
+        <v>75</v>
+      </c>
+      <c r="AV19" s="42" t="s">
+        <v>75</v>
+      </c>
+      <c r="AW19" s="42" t="s">
+        <v>75</v>
+      </c>
+      <c r="AX19" s="42" t="s">
+        <v>75</v>
+      </c>
+      <c r="AY19" s="42" t="s">
+        <v>75</v>
+      </c>
+      <c r="AZ19" s="42" t="s">
+        <v>75</v>
+      </c>
+      <c r="BA19" s="42" t="s">
+        <v>75</v>
+      </c>
+      <c r="BB19" s="42" t="s">
+        <v>75</v>
+      </c>
+      <c r="BC19" s="42" t="s">
+        <v>75</v>
+      </c>
+      <c r="BD19" s="42" t="s">
+        <v>75</v>
+      </c>
+      <c r="BE19" s="42" t="s">
+        <v>75</v>
+      </c>
+      <c r="BF19" s="42" t="s">
+        <v>75</v>
+      </c>
+      <c r="BG19" s="42" t="s">
+        <v>75</v>
+      </c>
+      <c r="BH19" s="42" t="s">
+        <v>75</v>
+      </c>
+      <c r="BI19" s="42" t="s">
+        <v>75</v>
+      </c>
+      <c r="BJ19" s="42" t="s">
+        <v>75</v>
+      </c>
+      <c r="BK19" s="42" t="s">
+        <v>75</v>
+      </c>
+      <c r="BL19" s="42" t="s">
+        <v>75</v>
+      </c>
+      <c r="BM19" s="42" t="s">
+        <v>75</v>
+      </c>
+      <c r="BN19" s="42" t="s">
+        <v>75</v>
+      </c>
+      <c r="BO19" s="42" t="s">
+        <v>75</v>
+      </c>
+      <c r="BP19" s="42" t="s">
+        <v>75</v>
+      </c>
+      <c r="BQ19" s="42" t="s">
+        <v>75</v>
+      </c>
       <c r="BR19" t="s">
         <v>75</v>
       </c>
@@ -6262,10 +6398,10 @@
         <v>163</v>
       </c>
       <c r="J21" s="3" t="s">
-        <v>368</v>
+        <v>172</v>
       </c>
       <c r="K21" s="3" t="s">
-        <v>368</v>
+        <v>172</v>
       </c>
       <c r="L21" t="s">
         <v>282</v>
@@ -6328,10 +6464,10 @@
         <v>163</v>
       </c>
       <c r="AF21" s="3" t="s">
-        <v>368</v>
+        <v>172</v>
       </c>
       <c r="AG21" s="3" t="s">
-        <v>368</v>
+        <v>172</v>
       </c>
       <c r="AH21" s="42" t="s">
         <v>171</v>
@@ -6343,7 +6479,7 @@
         <v>172</v>
       </c>
       <c r="AK21" s="3" t="s">
-        <v>368</v>
+        <v>172</v>
       </c>
       <c r="AL21" t="s">
         <v>171</v>
@@ -6400,16 +6536,16 @@
         <v>172</v>
       </c>
       <c r="BD21" t="s">
-        <v>368</v>
+        <v>172</v>
       </c>
       <c r="BE21" s="3" t="s">
-        <v>368</v>
+        <v>172</v>
       </c>
       <c r="BF21" t="s">
         <v>172</v>
       </c>
       <c r="BG21" t="s">
-        <v>368</v>
+        <v>172</v>
       </c>
       <c r="BH21" t="s">
         <v>171</v>
@@ -6418,7 +6554,7 @@
         <v>172</v>
       </c>
       <c r="BJ21" t="s">
-        <v>369</v>
+        <v>368</v>
       </c>
       <c r="BK21" s="42" t="s">
         <v>171</v>
@@ -6509,8 +6645,8 @@
       <c r="C22" t="s">
         <v>171</v>
       </c>
-      <c r="D22" s="3" t="s">
-        <v>368</v>
+      <c r="D22" s="58" t="s">
+        <v>172</v>
       </c>
       <c r="E22" s="58" t="s">
         <v>173</v>
@@ -6522,10 +6658,10 @@
         <v>282</v>
       </c>
       <c r="H22" s="3" t="s">
-        <v>368</v>
+        <v>172</v>
       </c>
       <c r="I22" s="3" t="s">
-        <v>368</v>
+        <v>172</v>
       </c>
       <c r="J22" t="s">
         <v>163</v>
@@ -6603,7 +6739,7 @@
         <v>171</v>
       </c>
       <c r="AI22" s="3" t="s">
-        <v>368</v>
+        <v>172</v>
       </c>
       <c r="AJ22" t="s">
         <v>163</v>
@@ -6914,7 +7050,7 @@
         <v>172</v>
       </c>
       <c r="AX23" s="3" t="s">
-        <v>368</v>
+        <v>172</v>
       </c>
       <c r="AY23" t="s">
         <v>171</v>
@@ -7123,7 +7259,7 @@
         <v>282</v>
       </c>
       <c r="AE24" s="3" t="s">
-        <v>368</v>
+        <v>172</v>
       </c>
       <c r="AF24" t="s">
         <v>163</v>
@@ -7153,7 +7289,7 @@
         <v>176</v>
       </c>
       <c r="AO24" s="3" t="s">
-        <v>368</v>
+        <v>172</v>
       </c>
       <c r="AP24" s="42" t="s">
         <v>171</v>
@@ -7452,7 +7588,7 @@
         <v>172</v>
       </c>
       <c r="AZ25" s="3" t="s">
-        <v>368</v>
+        <v>172</v>
       </c>
       <c r="BA25" t="s">
         <v>163</v>
@@ -7911,10 +8047,10 @@
         <v>2018</v>
       </c>
       <c r="F29" s="42" t="s">
-        <v>526</v>
+        <v>524</v>
       </c>
       <c r="G29" s="58" t="s">
-        <v>527</v>
+        <v>525</v>
       </c>
       <c r="H29" s="42">
         <v>2012</v>
@@ -7929,7 +8065,7 @@
         <v>2020</v>
       </c>
       <c r="M29" s="58" t="s">
-        <v>529</v>
+        <v>527</v>
       </c>
       <c r="N29">
         <v>2007</v>
@@ -7950,7 +8086,7 @@
         <v>2020</v>
       </c>
       <c r="T29" s="42" t="s">
-        <v>396</v>
+        <v>394</v>
       </c>
       <c r="U29" s="42">
         <v>1996</v>
@@ -7965,7 +8101,7 @@
         <v>2011</v>
       </c>
       <c r="Y29" s="42" t="s">
-        <v>397</v>
+        <v>395</v>
       </c>
       <c r="Z29" s="43">
         <v>1992</v>
@@ -7989,7 +8125,7 @@
         <v>2002</v>
       </c>
       <c r="AG29" s="58" t="s">
-        <v>399</v>
+        <v>397</v>
       </c>
       <c r="AH29">
         <v>2007</v>
@@ -8158,7 +8294,7 @@
         <v>2022</v>
       </c>
       <c r="H30" s="42" t="s">
-        <v>528</v>
+        <v>526</v>
       </c>
       <c r="I30" s="42"/>
       <c r="J30" s="42"/>
@@ -8166,7 +8302,7 @@
         <v>2021</v>
       </c>
       <c r="M30" s="58" t="s">
-        <v>395</v>
+        <v>393</v>
       </c>
       <c r="O30" s="42">
         <v>2008</v>
@@ -8183,7 +8319,7 @@
         <v>2002</v>
       </c>
       <c r="V30" s="42" t="s">
-        <v>395</v>
+        <v>393</v>
       </c>
       <c r="W30">
         <v>2010</v>
@@ -8192,19 +8328,19 @@
         <v>2018</v>
       </c>
       <c r="Y30" s="42" t="s">
-        <v>398</v>
+        <v>396</v>
       </c>
       <c r="Z30" s="43"/>
       <c r="AA30" s="43"/>
       <c r="AB30" s="58" t="s">
-        <v>395</v>
+        <v>393</v>
       </c>
       <c r="AC30">
         <v>2008</v>
       </c>
       <c r="AF30" s="42"/>
       <c r="AG30" s="58" t="s">
-        <v>400</v>
+        <v>398</v>
       </c>
       <c r="AI30" s="42"/>
       <c r="AK30" s="42">
@@ -8226,7 +8362,7 @@
         <v>1996</v>
       </c>
       <c r="AR30" s="42" t="s">
-        <v>395</v>
+        <v>393</v>
       </c>
       <c r="AS30" s="42">
         <v>2022</v>
@@ -8247,7 +8383,7 @@
       <c r="AZ30" s="42"/>
       <c r="BA30" s="42"/>
       <c r="BB30" s="42" t="s">
-        <v>395</v>
+        <v>393</v>
       </c>
       <c r="BC30" s="42"/>
       <c r="BE30" s="42"/>
@@ -8265,7 +8401,7 @@
         <v>2010</v>
       </c>
       <c r="BN30" s="42" t="s">
-        <v>395</v>
+        <v>393</v>
       </c>
       <c r="BQ30" s="42">
         <v>1998</v>
@@ -8281,7 +8417,7 @@
       </c>
       <c r="BV30" s="32"/>
       <c r="BW30" s="32" t="s">
-        <v>395</v>
+        <v>393</v>
       </c>
       <c r="BX30" s="32" t="s">
         <v>265</v>
@@ -8745,52 +8881,52 @@
         <v>163</v>
       </c>
       <c r="C35" t="s">
-        <v>530</v>
+        <v>528</v>
       </c>
       <c r="D35" t="s">
         <v>162</v>
       </c>
       <c r="E35" s="3" t="s">
-        <v>533</v>
+        <v>162</v>
       </c>
       <c r="F35" s="3" t="s">
-        <v>389</v>
+        <v>282</v>
       </c>
       <c r="G35" s="3" t="s">
-        <v>389</v>
+        <v>282</v>
       </c>
       <c r="H35" t="s">
         <v>162</v>
       </c>
       <c r="I35" t="s">
-        <v>389</v>
+        <v>282</v>
       </c>
       <c r="J35" s="3" t="s">
-        <v>533</v>
+        <v>162</v>
       </c>
       <c r="K35" s="3" t="s">
-        <v>389</v>
+        <v>282</v>
       </c>
       <c r="L35" s="3" t="s">
-        <v>389</v>
+        <v>282</v>
       </c>
       <c r="M35" s="58" t="s">
-        <v>531</v>
+        <v>529</v>
       </c>
       <c r="N35" t="s">
-        <v>532</v>
+        <v>530</v>
       </c>
       <c r="O35" t="s">
         <v>162</v>
       </c>
       <c r="P35" s="3" t="s">
-        <v>533</v>
+        <v>162</v>
       </c>
       <c r="Q35" t="s">
         <v>162</v>
       </c>
       <c r="R35" s="58" t="s">
-        <v>531</v>
+        <v>529</v>
       </c>
       <c r="S35" t="s">
         <v>163</v>
@@ -8799,19 +8935,19 @@
         <v>162</v>
       </c>
       <c r="U35" t="s">
-        <v>389</v>
+        <v>282</v>
       </c>
       <c r="V35" t="s">
-        <v>530</v>
+        <v>528</v>
       </c>
       <c r="W35" s="3" t="s">
-        <v>533</v>
+        <v>162</v>
       </c>
       <c r="X35" s="3" t="s">
-        <v>389</v>
+        <v>282</v>
       </c>
       <c r="Y35" s="3" t="s">
-        <v>389</v>
+        <v>282</v>
       </c>
       <c r="Z35" t="s">
         <v>162</v>
@@ -8820,40 +8956,40 @@
         <v>162</v>
       </c>
       <c r="AB35" t="s">
-        <v>530</v>
+        <v>528</v>
       </c>
       <c r="AC35" s="3" t="s">
-        <v>533</v>
+        <v>162</v>
       </c>
       <c r="AD35" s="3" t="s">
-        <v>389</v>
+        <v>282</v>
       </c>
       <c r="AE35" s="3" t="s">
-        <v>533</v>
+        <v>162</v>
       </c>
       <c r="AF35" t="s">
         <v>163</v>
       </c>
       <c r="AG35" s="58" t="s">
-        <v>531</v>
+        <v>529</v>
       </c>
       <c r="AH35" s="3" t="s">
-        <v>533</v>
+        <v>162</v>
       </c>
       <c r="AI35" t="s">
+        <v>528</v>
+      </c>
+      <c r="AJ35" t="s">
         <v>530</v>
-      </c>
-      <c r="AJ35" t="s">
-        <v>532</v>
       </c>
       <c r="AK35" t="s">
         <v>282</v>
       </c>
       <c r="AL35" t="s">
-        <v>532</v>
+        <v>530</v>
       </c>
       <c r="AM35" t="s">
-        <v>532</v>
+        <v>530</v>
       </c>
       <c r="AN35" t="s">
         <v>162</v>
@@ -8862,40 +8998,40 @@
         <v>162</v>
       </c>
       <c r="AP35" s="58" t="s">
-        <v>531</v>
+        <v>529</v>
       </c>
       <c r="AQ35" t="s">
-        <v>389</v>
+        <v>282</v>
       </c>
       <c r="AR35" t="s">
         <v>162</v>
       </c>
       <c r="AS35" t="s">
-        <v>532</v>
+        <v>530</v>
       </c>
       <c r="AT35" t="s">
-        <v>532</v>
+        <v>530</v>
       </c>
       <c r="AU35" t="s">
-        <v>532</v>
+        <v>530</v>
       </c>
       <c r="AV35" t="s">
-        <v>532</v>
+        <v>530</v>
       </c>
       <c r="AW35" t="s">
         <v>162</v>
       </c>
       <c r="AX35" t="s">
-        <v>530</v>
+        <v>528</v>
       </c>
       <c r="AY35" s="3" t="s">
-        <v>533</v>
+        <v>162</v>
       </c>
       <c r="AZ35" s="3" t="s">
-        <v>533</v>
+        <v>162</v>
       </c>
       <c r="BA35" t="s">
-        <v>530</v>
+        <v>528</v>
       </c>
       <c r="BB35" t="s">
         <v>162</v>
@@ -8904,7 +9040,7 @@
         <v>162</v>
       </c>
       <c r="BD35" t="s">
-        <v>532</v>
+        <v>530</v>
       </c>
       <c r="BE35" t="s">
         <v>162</v>
@@ -8913,10 +9049,10 @@
         <v>162</v>
       </c>
       <c r="BG35" t="s">
-        <v>533</v>
+        <v>162</v>
       </c>
       <c r="BH35" t="s">
-        <v>532</v>
+        <v>530</v>
       </c>
       <c r="BI35" t="s">
         <v>162</v>
@@ -8931,7 +9067,7 @@
         <v>162</v>
       </c>
       <c r="BM35" s="3" t="s">
-        <v>533</v>
+        <v>162</v>
       </c>
       <c r="BN35" t="s">
         <v>162</v>
@@ -9011,76 +9147,76 @@
         <v>162</v>
       </c>
       <c r="C36" t="s">
-        <v>530</v>
+        <v>528</v>
       </c>
       <c r="D36" t="s">
         <v>163</v>
       </c>
       <c r="E36" s="3" t="s">
-        <v>533</v>
+        <v>162</v>
       </c>
       <c r="F36" s="3" t="s">
-        <v>389</v>
+        <v>282</v>
       </c>
       <c r="G36" s="3" t="s">
-        <v>389</v>
+        <v>282</v>
       </c>
       <c r="H36" t="s">
         <v>162</v>
       </c>
       <c r="I36" t="s">
-        <v>389</v>
+        <v>282</v>
       </c>
       <c r="J36" s="3" t="s">
-        <v>533</v>
+        <v>162</v>
       </c>
       <c r="K36" s="3" t="s">
-        <v>389</v>
+        <v>282</v>
       </c>
       <c r="L36" s="3" t="s">
-        <v>389</v>
+        <v>282</v>
       </c>
       <c r="M36" s="58" t="s">
-        <v>531</v>
+        <v>529</v>
       </c>
       <c r="N36" s="58" t="s">
-        <v>531</v>
+        <v>529</v>
       </c>
       <c r="O36" t="s">
-        <v>530</v>
+        <v>528</v>
       </c>
       <c r="P36" s="3" t="s">
-        <v>533</v>
+        <v>162</v>
       </c>
       <c r="Q36" t="s">
         <v>163</v>
       </c>
       <c r="R36" t="s">
-        <v>530</v>
+        <v>528</v>
       </c>
       <c r="S36" t="s">
-        <v>530</v>
+        <v>528</v>
       </c>
       <c r="T36" t="s">
-        <v>530</v>
+        <v>528</v>
       </c>
       <c r="U36" t="s">
-        <v>389</v>
+        <v>282</v>
       </c>
       <c r="V36" t="s">
-        <v>530</v>
+        <v>528</v>
       </c>
       <c r="W36" t="s">
         <v>162</v>
       </c>
       <c r="X36" t="s">
-        <v>389</v>
+        <v>282</v>
       </c>
       <c r="Y36" t="s">
-        <v>389</v>
+        <v>282</v>
       </c>
       <c r="Z36" t="s">
-        <v>532</v>
+        <v>530</v>
       </c>
       <c r="AA36" s="5" t="s">
         <v>163</v>
@@ -9089,79 +9225,79 @@
         <v>162</v>
       </c>
       <c r="AC36" t="s">
-        <v>530</v>
+        <v>528</v>
       </c>
       <c r="AD36" t="s">
-        <v>389</v>
+        <v>282</v>
       </c>
       <c r="AE36" s="58" t="s">
-        <v>531</v>
+        <v>529</v>
       </c>
       <c r="AF36" t="s">
         <v>163</v>
       </c>
       <c r="AG36" t="s">
+        <v>528</v>
+      </c>
+      <c r="AH36" s="3" t="s">
+        <v>162</v>
+      </c>
+      <c r="AI36" t="s">
+        <v>528</v>
+      </c>
+      <c r="AJ36" t="s">
+        <v>528</v>
+      </c>
+      <c r="AK36" s="3" t="s">
+        <v>162</v>
+      </c>
+      <c r="AL36" t="s">
         <v>530</v>
       </c>
-      <c r="AH36" s="3" t="s">
-        <v>533</v>
-      </c>
-      <c r="AI36" t="s">
-        <v>530</v>
-      </c>
-      <c r="AJ36" t="s">
-        <v>530</v>
-      </c>
-      <c r="AK36" s="3" t="s">
-        <v>533</v>
-      </c>
-      <c r="AL36" t="s">
-        <v>532</v>
-      </c>
       <c r="AM36" t="s">
-        <v>530</v>
+        <v>528</v>
       </c>
       <c r="AN36" s="58" t="s">
-        <v>531</v>
+        <v>529</v>
       </c>
       <c r="AO36" t="s">
         <v>162</v>
       </c>
       <c r="AP36" s="58" t="s">
-        <v>531</v>
+        <v>529</v>
       </c>
       <c r="AQ36" t="s">
-        <v>389</v>
+        <v>282</v>
       </c>
       <c r="AR36" t="s">
-        <v>530</v>
+        <v>528</v>
       </c>
       <c r="AS36" t="s">
-        <v>530</v>
+        <v>528</v>
       </c>
       <c r="AT36" t="s">
-        <v>530</v>
+        <v>528</v>
       </c>
       <c r="AU36" t="s">
-        <v>530</v>
+        <v>528</v>
       </c>
       <c r="AV36" s="58" t="s">
-        <v>531</v>
+        <v>529</v>
       </c>
       <c r="AW36" t="s">
         <v>162</v>
       </c>
       <c r="AX36" s="58" t="s">
-        <v>531</v>
+        <v>529</v>
       </c>
       <c r="AY36" t="s">
         <v>162</v>
       </c>
       <c r="AZ36" s="3" t="s">
-        <v>533</v>
+        <v>162</v>
       </c>
       <c r="BA36" t="s">
-        <v>530</v>
+        <v>528</v>
       </c>
       <c r="BB36" t="s">
         <v>162</v>
@@ -9170,40 +9306,40 @@
         <v>162</v>
       </c>
       <c r="BD36" t="s">
-        <v>530</v>
+        <v>528</v>
       </c>
       <c r="BE36" t="s">
         <v>162</v>
       </c>
       <c r="BF36" t="s">
-        <v>532</v>
+        <v>530</v>
       </c>
       <c r="BG36" t="s">
-        <v>532</v>
+        <v>530</v>
       </c>
       <c r="BH36" t="s">
-        <v>532</v>
+        <v>530</v>
       </c>
       <c r="BI36" t="s">
-        <v>530</v>
+        <v>528</v>
       </c>
       <c r="BJ36" t="s">
         <v>162</v>
       </c>
       <c r="BK36" t="s">
-        <v>530</v>
+        <v>528</v>
       </c>
       <c r="BL36" t="s">
         <v>162</v>
       </c>
       <c r="BM36" s="3" t="s">
-        <v>533</v>
+        <v>162</v>
       </c>
       <c r="BN36" t="s">
         <v>162</v>
       </c>
       <c r="BO36" s="58" t="s">
-        <v>531</v>
+        <v>529</v>
       </c>
       <c r="BP36" t="s">
         <v>163</v>
@@ -9274,82 +9410,82 @@
         <v>186</v>
       </c>
       <c r="B37" t="s">
-        <v>530</v>
+        <v>528</v>
       </c>
       <c r="C37" t="s">
-        <v>530</v>
+        <v>528</v>
       </c>
       <c r="D37" t="s">
-        <v>389</v>
+        <v>282</v>
       </c>
       <c r="E37" s="3" t="s">
-        <v>533</v>
+        <v>162</v>
       </c>
       <c r="F37" s="3" t="s">
-        <v>389</v>
+        <v>282</v>
       </c>
       <c r="G37" s="3" t="s">
-        <v>389</v>
+        <v>282</v>
       </c>
       <c r="H37" t="s">
-        <v>530</v>
+        <v>528</v>
       </c>
       <c r="I37" t="s">
-        <v>389</v>
+        <v>282</v>
       </c>
       <c r="J37" s="3" t="s">
-        <v>533</v>
+        <v>162</v>
       </c>
       <c r="K37" s="3" t="s">
-        <v>389</v>
+        <v>282</v>
       </c>
       <c r="L37" s="3" t="s">
-        <v>389</v>
+        <v>282</v>
       </c>
       <c r="M37" t="s">
-        <v>530</v>
+        <v>528</v>
       </c>
       <c r="N37" t="s">
-        <v>530</v>
+        <v>528</v>
       </c>
       <c r="O37" t="s">
-        <v>389</v>
+        <v>282</v>
       </c>
       <c r="P37" t="s">
-        <v>530</v>
+        <v>528</v>
       </c>
       <c r="Q37" t="s">
-        <v>389</v>
+        <v>282</v>
       </c>
       <c r="R37" t="s">
-        <v>530</v>
+        <v>528</v>
       </c>
       <c r="S37" t="s">
         <v>163</v>
       </c>
       <c r="T37" t="s">
-        <v>530</v>
+        <v>528</v>
       </c>
       <c r="U37" t="s">
-        <v>389</v>
+        <v>282</v>
       </c>
       <c r="V37" t="s">
-        <v>530</v>
+        <v>528</v>
       </c>
       <c r="W37" t="s">
-        <v>530</v>
+        <v>528</v>
       </c>
       <c r="X37" t="s">
-        <v>389</v>
+        <v>282</v>
       </c>
       <c r="Y37" t="s">
-        <v>389</v>
+        <v>282</v>
       </c>
       <c r="Z37" t="s">
         <v>163</v>
       </c>
       <c r="AA37" s="5" t="s">
-        <v>389</v>
+        <v>282</v>
       </c>
       <c r="AB37" t="s">
         <v>163</v>
@@ -9358,25 +9494,25 @@
         <v>163</v>
       </c>
       <c r="AD37" t="s">
-        <v>389</v>
+        <v>282</v>
       </c>
       <c r="AE37" t="s">
-        <v>530</v>
+        <v>528</v>
       </c>
       <c r="AF37" t="s">
-        <v>389</v>
+        <v>282</v>
       </c>
       <c r="AG37" t="s">
-        <v>530</v>
+        <v>528</v>
       </c>
       <c r="AH37" t="s">
-        <v>530</v>
+        <v>528</v>
       </c>
       <c r="AI37" t="s">
         <v>163</v>
       </c>
       <c r="AJ37" t="s">
-        <v>530</v>
+        <v>528</v>
       </c>
       <c r="AK37" t="s">
         <v>163</v>
@@ -9388,22 +9524,22 @@
         <v>163</v>
       </c>
       <c r="AN37" t="s">
-        <v>389</v>
+        <v>282</v>
       </c>
       <c r="AO37" t="s">
-        <v>530</v>
+        <v>528</v>
       </c>
       <c r="AP37" t="s">
-        <v>530</v>
+        <v>528</v>
       </c>
       <c r="AQ37" t="s">
-        <v>389</v>
+        <v>282</v>
       </c>
       <c r="AR37" t="s">
-        <v>530</v>
+        <v>528</v>
       </c>
       <c r="AS37" t="s">
-        <v>389</v>
+        <v>282</v>
       </c>
       <c r="AT37" t="s">
         <v>163</v>
@@ -9412,40 +9548,40 @@
         <v>163</v>
       </c>
       <c r="AV37" s="58" t="s">
-        <v>531</v>
+        <v>529</v>
       </c>
       <c r="AW37" t="s">
-        <v>530</v>
+        <v>528</v>
       </c>
       <c r="AX37" t="s">
         <v>163</v>
       </c>
       <c r="AY37" t="s">
-        <v>532</v>
+        <v>530</v>
       </c>
       <c r="AZ37" s="3" t="s">
-        <v>533</v>
+        <v>162</v>
       </c>
       <c r="BA37" t="s">
         <v>163</v>
       </c>
       <c r="BB37" t="s">
-        <v>530</v>
+        <v>528</v>
       </c>
       <c r="BC37" t="s">
         <v>162</v>
       </c>
       <c r="BD37" t="s">
-        <v>530</v>
+        <v>528</v>
       </c>
       <c r="BE37" t="s">
-        <v>389</v>
+        <v>282</v>
       </c>
       <c r="BF37" t="s">
-        <v>530</v>
+        <v>528</v>
       </c>
       <c r="BG37" t="s">
-        <v>530</v>
+        <v>528</v>
       </c>
       <c r="BH37" t="s">
         <v>282</v>
@@ -9454,7 +9590,7 @@
         <v>163</v>
       </c>
       <c r="BJ37" t="s">
-        <v>532</v>
+        <v>530</v>
       </c>
       <c r="BK37" t="s">
         <v>163</v>
@@ -9463,10 +9599,10 @@
         <v>162</v>
       </c>
       <c r="BM37" s="3" t="s">
-        <v>533</v>
+        <v>162</v>
       </c>
       <c r="BN37" t="s">
-        <v>530</v>
+        <v>528</v>
       </c>
       <c r="BO37" t="s">
         <v>163</v>
@@ -9540,82 +9676,82 @@
         <v>187</v>
       </c>
       <c r="B38" t="s">
-        <v>530</v>
+        <v>528</v>
       </c>
       <c r="C38" t="s">
         <v>163</v>
       </c>
       <c r="D38" t="s">
-        <v>389</v>
+        <v>282</v>
       </c>
       <c r="E38" t="s">
         <v>163</v>
       </c>
       <c r="F38" s="3" t="s">
-        <v>389</v>
+        <v>282</v>
       </c>
       <c r="G38" s="3" t="s">
-        <v>389</v>
+        <v>282</v>
       </c>
       <c r="H38" t="s">
-        <v>530</v>
+        <v>528</v>
       </c>
       <c r="I38" t="s">
-        <v>389</v>
+        <v>282</v>
       </c>
       <c r="J38" s="58" t="s">
-        <v>531</v>
+        <v>529</v>
       </c>
       <c r="K38" s="3" t="s">
-        <v>389</v>
+        <v>282</v>
       </c>
       <c r="L38" s="3" t="s">
-        <v>389</v>
+        <v>282</v>
       </c>
       <c r="M38" t="s">
-        <v>530</v>
+        <v>528</v>
       </c>
       <c r="N38" t="s">
-        <v>530</v>
+        <v>528</v>
       </c>
       <c r="O38" t="s">
-        <v>389</v>
+        <v>282</v>
       </c>
       <c r="P38" s="58" t="s">
-        <v>531</v>
+        <v>529</v>
       </c>
       <c r="Q38" t="s">
-        <v>389</v>
+        <v>282</v>
       </c>
       <c r="R38" t="s">
-        <v>530</v>
+        <v>528</v>
       </c>
       <c r="S38" t="s">
         <v>163</v>
       </c>
       <c r="T38" t="s">
-        <v>530</v>
+        <v>528</v>
       </c>
       <c r="U38" t="s">
-        <v>389</v>
+        <v>282</v>
       </c>
       <c r="V38" t="s">
-        <v>530</v>
+        <v>528</v>
       </c>
       <c r="W38" t="s">
         <v>163</v>
       </c>
       <c r="X38" t="s">
-        <v>389</v>
+        <v>282</v>
       </c>
       <c r="Y38" t="s">
-        <v>389</v>
+        <v>282</v>
       </c>
       <c r="Z38" t="s">
         <v>163</v>
       </c>
       <c r="AA38" s="5" t="s">
-        <v>389</v>
+        <v>282</v>
       </c>
       <c r="AB38" t="s">
         <v>162</v>
@@ -9624,64 +9760,64 @@
         <v>163</v>
       </c>
       <c r="AD38" t="s">
-        <v>389</v>
+        <v>282</v>
       </c>
       <c r="AE38" s="58" t="s">
-        <v>531</v>
+        <v>529</v>
       </c>
       <c r="AF38" t="s">
-        <v>389</v>
+        <v>282</v>
       </c>
       <c r="AG38" t="s">
         <v>282</v>
       </c>
       <c r="AH38" t="s">
-        <v>530</v>
+        <v>528</v>
       </c>
       <c r="AI38" t="s">
         <v>163</v>
       </c>
       <c r="AJ38" t="s">
-        <v>530</v>
+        <v>528</v>
       </c>
       <c r="AK38" t="s">
         <v>163</v>
       </c>
       <c r="AL38" t="s">
-        <v>530</v>
+        <v>528</v>
       </c>
       <c r="AM38" t="s">
         <v>163</v>
       </c>
       <c r="AN38" t="s">
-        <v>389</v>
+        <v>282</v>
       </c>
       <c r="AO38" t="s">
         <v>162</v>
       </c>
       <c r="AP38" t="s">
-        <v>530</v>
+        <v>528</v>
       </c>
       <c r="AQ38" t="s">
-        <v>389</v>
+        <v>282</v>
       </c>
       <c r="AR38" t="s">
         <v>163</v>
       </c>
       <c r="AS38" t="s">
-        <v>389</v>
+        <v>282</v>
       </c>
       <c r="AT38" t="s">
-        <v>530</v>
+        <v>528</v>
       </c>
       <c r="AU38" t="s">
-        <v>530</v>
+        <v>528</v>
       </c>
       <c r="AV38" t="s">
         <v>163</v>
       </c>
       <c r="AW38" t="s">
-        <v>530</v>
+        <v>528</v>
       </c>
       <c r="AX38" t="s">
         <v>163</v>
@@ -9696,28 +9832,28 @@
         <v>163</v>
       </c>
       <c r="BB38" t="s">
-        <v>530</v>
+        <v>528</v>
       </c>
       <c r="BC38" t="s">
         <v>163</v>
       </c>
       <c r="BD38" t="s">
+        <v>528</v>
+      </c>
+      <c r="BE38" t="s">
+        <v>282</v>
+      </c>
+      <c r="BF38" t="s">
         <v>530</v>
-      </c>
-      <c r="BE38" t="s">
-        <v>389</v>
-      </c>
-      <c r="BF38" t="s">
-        <v>532</v>
       </c>
       <c r="BG38" t="s">
         <v>163</v>
       </c>
       <c r="BH38" t="s">
-        <v>532</v>
+        <v>530</v>
       </c>
       <c r="BI38" t="s">
-        <v>530</v>
+        <v>528</v>
       </c>
       <c r="BJ38" t="s">
         <v>163</v>
@@ -9729,10 +9865,10 @@
         <v>282</v>
       </c>
       <c r="BM38" s="3" t="s">
-        <v>533</v>
+        <v>162</v>
       </c>
       <c r="BN38" t="s">
-        <v>530</v>
+        <v>528</v>
       </c>
       <c r="BO38" t="s">
         <v>163</v>
@@ -9812,76 +9948,76 @@
         <v>163</v>
       </c>
       <c r="D39" t="s">
-        <v>389</v>
+        <v>282</v>
       </c>
       <c r="E39" s="3" t="s">
-        <v>533</v>
+        <v>162</v>
       </c>
       <c r="F39" s="3" t="s">
-        <v>389</v>
+        <v>282</v>
       </c>
       <c r="G39" s="3" t="s">
-        <v>389</v>
+        <v>282</v>
       </c>
       <c r="H39" t="s">
         <v>162</v>
       </c>
       <c r="I39" t="s">
-        <v>389</v>
+        <v>282</v>
       </c>
       <c r="J39" t="s">
         <v>163</v>
       </c>
       <c r="K39" s="3" t="s">
-        <v>389</v>
+        <v>282</v>
       </c>
       <c r="L39" s="3" t="s">
-        <v>389</v>
+        <v>282</v>
       </c>
       <c r="M39" t="s">
-        <v>530</v>
+        <v>528</v>
       </c>
       <c r="N39" t="s">
-        <v>530</v>
+        <v>528</v>
       </c>
       <c r="O39" t="s">
-        <v>389</v>
+        <v>282</v>
       </c>
       <c r="P39" t="s">
         <v>162</v>
       </c>
       <c r="Q39" t="s">
-        <v>389</v>
+        <v>282</v>
       </c>
       <c r="R39" t="s">
-        <v>530</v>
+        <v>528</v>
       </c>
       <c r="S39" t="s">
-        <v>530</v>
+        <v>528</v>
       </c>
       <c r="T39" t="s">
-        <v>530</v>
+        <v>528</v>
       </c>
       <c r="U39" t="s">
-        <v>389</v>
+        <v>282</v>
       </c>
       <c r="V39" t="s">
-        <v>530</v>
+        <v>528</v>
       </c>
       <c r="W39" t="s">
         <v>162</v>
       </c>
       <c r="X39" t="s">
-        <v>389</v>
+        <v>282</v>
       </c>
       <c r="Y39" t="s">
-        <v>389</v>
+        <v>282</v>
       </c>
       <c r="Z39" t="s">
-        <v>532</v>
+        <v>530</v>
       </c>
       <c r="AA39" s="5" t="s">
-        <v>389</v>
+        <v>282</v>
       </c>
       <c r="AB39" t="s">
         <v>162</v>
@@ -9890,58 +10026,58 @@
         <v>163</v>
       </c>
       <c r="AD39" t="s">
-        <v>389</v>
+        <v>282</v>
       </c>
       <c r="AE39" t="s">
         <v>163</v>
       </c>
       <c r="AF39" t="s">
-        <v>389</v>
+        <v>282</v>
       </c>
       <c r="AG39" t="s">
-        <v>530</v>
+        <v>528</v>
       </c>
       <c r="AH39" t="s">
         <v>162</v>
       </c>
       <c r="AI39" t="s">
+        <v>528</v>
+      </c>
+      <c r="AJ39" t="s">
+        <v>528</v>
+      </c>
+      <c r="AK39" s="3" t="s">
+        <v>162</v>
+      </c>
+      <c r="AL39" t="s">
         <v>530</v>
-      </c>
-      <c r="AJ39" t="s">
-        <v>530</v>
-      </c>
-      <c r="AK39" s="3" t="s">
-        <v>533</v>
-      </c>
-      <c r="AL39" t="s">
-        <v>532</v>
       </c>
       <c r="AM39" t="s">
         <v>163</v>
       </c>
       <c r="AN39" t="s">
-        <v>389</v>
+        <v>282</v>
       </c>
       <c r="AO39" t="s">
         <v>162</v>
       </c>
       <c r="AP39" t="s">
-        <v>531</v>
+        <v>529</v>
       </c>
       <c r="AQ39" t="s">
-        <v>389</v>
+        <v>282</v>
       </c>
       <c r="AR39" t="s">
-        <v>530</v>
+        <v>528</v>
       </c>
       <c r="AS39" t="s">
-        <v>389</v>
+        <v>282</v>
       </c>
       <c r="AT39" t="s">
-        <v>530</v>
+        <v>528</v>
       </c>
       <c r="AU39" t="s">
-        <v>530</v>
+        <v>528</v>
       </c>
       <c r="AV39" t="s">
         <v>163</v>
@@ -9950,40 +10086,40 @@
         <v>162</v>
       </c>
       <c r="AX39" s="58" t="s">
-        <v>531</v>
+        <v>529</v>
       </c>
       <c r="AY39" t="s">
-        <v>532</v>
+        <v>530</v>
       </c>
       <c r="AZ39" t="s">
-        <v>532</v>
+        <v>530</v>
       </c>
       <c r="BA39" t="s">
-        <v>530</v>
+        <v>528</v>
       </c>
       <c r="BB39" t="s">
         <v>162</v>
       </c>
       <c r="BC39" t="s">
+        <v>528</v>
+      </c>
+      <c r="BD39" t="s">
+        <v>529</v>
+      </c>
+      <c r="BE39" t="s">
+        <v>282</v>
+      </c>
+      <c r="BF39" t="s">
         <v>530</v>
       </c>
-      <c r="BD39" t="s">
-        <v>531</v>
-      </c>
-      <c r="BE39" t="s">
-        <v>389</v>
-      </c>
-      <c r="BF39" t="s">
-        <v>532</v>
-      </c>
       <c r="BG39" t="s">
-        <v>532</v>
+        <v>530</v>
       </c>
       <c r="BH39" t="s">
-        <v>532</v>
+        <v>530</v>
       </c>
       <c r="BI39" t="s">
-        <v>530</v>
+        <v>528</v>
       </c>
       <c r="BJ39" t="s">
         <v>162</v>
@@ -9995,13 +10131,13 @@
         <v>162</v>
       </c>
       <c r="BM39" s="3" t="s">
-        <v>533</v>
+        <v>162</v>
       </c>
       <c r="BN39" t="s">
         <v>162</v>
       </c>
       <c r="BO39" s="58" t="s">
-        <v>531</v>
+        <v>529</v>
       </c>
       <c r="BP39" t="s">
         <v>163</v>
@@ -10075,49 +10211,49 @@
         <v>282</v>
       </c>
       <c r="C40" t="s">
-        <v>389</v>
+        <v>282</v>
       </c>
       <c r="D40" t="s">
-        <v>389</v>
+        <v>282</v>
       </c>
       <c r="E40" t="s">
-        <v>370</v>
+        <v>369</v>
       </c>
       <c r="F40" s="3" t="s">
-        <v>389</v>
+        <v>282</v>
       </c>
       <c r="G40" s="3" t="s">
-        <v>389</v>
+        <v>282</v>
       </c>
       <c r="H40" s="3" t="s">
-        <v>389</v>
+        <v>282</v>
       </c>
       <c r="I40" s="3" t="s">
-        <v>389</v>
+        <v>282</v>
       </c>
       <c r="J40" t="s">
         <v>163</v>
       </c>
       <c r="K40" s="3" t="s">
-        <v>389</v>
+        <v>282</v>
       </c>
       <c r="L40" s="3" t="s">
-        <v>389</v>
+        <v>282</v>
       </c>
       <c r="M40" t="s">
         <v>163</v>
       </c>
       <c r="N40" t="s">
-        <v>530</v>
+        <v>528</v>
       </c>
       <c r="O40" t="s">
-        <v>389</v>
+        <v>282</v>
       </c>
       <c r="P40" t="s">
-        <v>530</v>
+        <v>528</v>
       </c>
       <c r="Q40" t="s">
-        <v>389</v>
+        <v>282</v>
       </c>
       <c r="R40" t="s">
         <v>163</v>
@@ -10129,7 +10265,7 @@
         <v>163</v>
       </c>
       <c r="U40" t="s">
-        <v>389</v>
+        <v>282</v>
       </c>
       <c r="V40" t="s">
         <v>163</v>
@@ -10138,16 +10274,16 @@
         <v>163</v>
       </c>
       <c r="X40" t="s">
-        <v>389</v>
+        <v>282</v>
       </c>
       <c r="Y40" t="s">
-        <v>389</v>
+        <v>282</v>
       </c>
       <c r="Z40" t="s">
-        <v>530</v>
+        <v>528</v>
       </c>
       <c r="AA40" s="5" t="s">
-        <v>389</v>
+        <v>282</v>
       </c>
       <c r="AB40" t="s">
         <v>163</v>
@@ -10156,13 +10292,13 @@
         <v>163</v>
       </c>
       <c r="AD40" t="s">
-        <v>389</v>
+        <v>282</v>
       </c>
       <c r="AE40" t="s">
-        <v>530</v>
+        <v>528</v>
       </c>
       <c r="AF40" t="s">
-        <v>389</v>
+        <v>282</v>
       </c>
       <c r="AG40" t="s">
         <v>282</v>
@@ -10174,19 +10310,19 @@
         <v>163</v>
       </c>
       <c r="AJ40" t="s">
-        <v>389</v>
+        <v>282</v>
       </c>
       <c r="AK40" t="s">
         <v>163</v>
       </c>
       <c r="AL40" t="s">
-        <v>389</v>
+        <v>282</v>
       </c>
       <c r="AM40" t="s">
         <v>163</v>
       </c>
       <c r="AN40" t="s">
-        <v>389</v>
+        <v>282</v>
       </c>
       <c r="AO40" t="s">
         <v>163</v>
@@ -10195,19 +10331,19 @@
         <v>163</v>
       </c>
       <c r="AQ40" t="s">
-        <v>389</v>
+        <v>282</v>
       </c>
       <c r="AR40" t="s">
-        <v>389</v>
+        <v>282</v>
       </c>
       <c r="AS40" t="s">
-        <v>389</v>
+        <v>282</v>
       </c>
       <c r="AT40" t="s">
-        <v>389</v>
+        <v>282</v>
       </c>
       <c r="AU40" t="s">
-        <v>389</v>
+        <v>282</v>
       </c>
       <c r="AV40" t="s">
         <v>163</v>
@@ -10228,22 +10364,22 @@
         <v>163</v>
       </c>
       <c r="BB40" t="s">
-        <v>389</v>
+        <v>282</v>
       </c>
       <c r="BC40" t="s">
-        <v>389</v>
+        <v>282</v>
       </c>
       <c r="BD40" t="s">
-        <v>389</v>
+        <v>282</v>
       </c>
       <c r="BE40" t="s">
-        <v>389</v>
+        <v>282</v>
       </c>
       <c r="BF40" t="s">
         <v>163</v>
       </c>
       <c r="BG40" t="s">
-        <v>530</v>
+        <v>528</v>
       </c>
       <c r="BH40" t="s">
         <v>282</v>
@@ -10255,19 +10391,19 @@
         <v>163</v>
       </c>
       <c r="BK40" t="s">
-        <v>389</v>
+        <v>282</v>
       </c>
       <c r="BL40" t="s">
         <v>163</v>
       </c>
       <c r="BM40" s="3" t="s">
-        <v>389</v>
+        <v>282</v>
       </c>
       <c r="BN40" t="s">
-        <v>530</v>
+        <v>528</v>
       </c>
       <c r="BO40" t="s">
-        <v>389</v>
+        <v>282</v>
       </c>
       <c r="BP40" t="s">
         <v>163</v>
@@ -10344,34 +10480,34 @@
         <v>162</v>
       </c>
       <c r="D41" s="3" t="s">
-        <v>533</v>
+        <v>162</v>
       </c>
       <c r="E41" s="3" t="s">
-        <v>533</v>
+        <v>162</v>
       </c>
       <c r="F41" s="3" t="s">
-        <v>389</v>
+        <v>282</v>
       </c>
       <c r="G41" s="3" t="s">
-        <v>389</v>
+        <v>282</v>
       </c>
       <c r="H41" s="3" t="s">
-        <v>533</v>
+        <v>162</v>
       </c>
       <c r="I41" s="3" t="s">
-        <v>389</v>
+        <v>282</v>
       </c>
       <c r="J41" s="3" t="s">
-        <v>533</v>
+        <v>162</v>
       </c>
       <c r="K41" s="3" t="s">
-        <v>389</v>
+        <v>282</v>
       </c>
       <c r="L41" s="3" t="s">
-        <v>389</v>
+        <v>282</v>
       </c>
       <c r="M41" s="3" t="s">
-        <v>533</v>
+        <v>162</v>
       </c>
       <c r="N41" t="s">
         <v>162</v>
@@ -10380,7 +10516,7 @@
         <v>162</v>
       </c>
       <c r="P41" s="3" t="s">
-        <v>533</v>
+        <v>162</v>
       </c>
       <c r="Q41" t="s">
         <v>163</v>
@@ -10395,19 +10531,19 @@
         <v>162</v>
       </c>
       <c r="U41" t="s">
-        <v>389</v>
+        <v>282</v>
       </c>
       <c r="V41" s="3" t="s">
-        <v>533</v>
+        <v>162</v>
       </c>
       <c r="W41" s="3" t="s">
-        <v>533</v>
+        <v>162</v>
       </c>
       <c r="X41" s="3" t="s">
-        <v>389</v>
+        <v>282</v>
       </c>
       <c r="Y41" s="3" t="s">
-        <v>389</v>
+        <v>282</v>
       </c>
       <c r="Z41" t="s">
         <v>162</v>
@@ -10419,13 +10555,13 @@
         <v>162</v>
       </c>
       <c r="AC41" s="3" t="s">
-        <v>533</v>
+        <v>162</v>
       </c>
       <c r="AD41" s="3" t="s">
-        <v>389</v>
+        <v>282</v>
       </c>
       <c r="AE41" s="3" t="s">
-        <v>533</v>
+        <v>162</v>
       </c>
       <c r="AF41" t="s">
         <v>163</v>
@@ -10434,64 +10570,64 @@
         <v>162</v>
       </c>
       <c r="AH41" s="3" t="s">
-        <v>533</v>
+        <v>162</v>
       </c>
       <c r="AI41" s="3" t="s">
-        <v>533</v>
+        <v>162</v>
       </c>
       <c r="AJ41" s="58" t="s">
-        <v>531</v>
+        <v>529</v>
       </c>
       <c r="AK41" s="3" t="s">
-        <v>533</v>
+        <v>162</v>
       </c>
       <c r="AL41" s="3" t="s">
-        <v>533</v>
+        <v>162</v>
       </c>
       <c r="AM41" s="3" t="s">
-        <v>533</v>
+        <v>162</v>
       </c>
       <c r="AN41" t="s">
         <v>162</v>
       </c>
       <c r="AO41" s="3" t="s">
-        <v>533</v>
+        <v>162</v>
       </c>
       <c r="AP41" t="s">
         <v>162</v>
       </c>
       <c r="AQ41" t="s">
-        <v>389</v>
+        <v>282</v>
       </c>
       <c r="AR41" t="s">
         <v>162</v>
       </c>
       <c r="AS41" t="s">
-        <v>532</v>
+        <v>530</v>
       </c>
       <c r="AT41" s="3" t="s">
-        <v>533</v>
+        <v>162</v>
       </c>
       <c r="AU41" s="3" t="s">
-        <v>533</v>
+        <v>162</v>
       </c>
       <c r="AV41" s="3" t="s">
-        <v>533</v>
+        <v>162</v>
       </c>
       <c r="AW41" t="s">
         <v>162</v>
       </c>
       <c r="AX41" s="3" t="s">
-        <v>533</v>
+        <v>162</v>
       </c>
       <c r="AY41" s="3" t="s">
-        <v>533</v>
+        <v>162</v>
       </c>
       <c r="AZ41" s="3" t="s">
-        <v>533</v>
+        <v>162</v>
       </c>
       <c r="BA41" s="3" t="s">
-        <v>533</v>
+        <v>162</v>
       </c>
       <c r="BB41" t="s">
         <v>162</v>
@@ -10500,7 +10636,7 @@
         <v>162</v>
       </c>
       <c r="BD41" t="s">
-        <v>533</v>
+        <v>162</v>
       </c>
       <c r="BE41" t="s">
         <v>162</v>
@@ -10509,10 +10645,10 @@
         <v>162</v>
       </c>
       <c r="BG41" t="s">
-        <v>533</v>
+        <v>162</v>
       </c>
       <c r="BH41" s="3" t="s">
-        <v>533</v>
+        <v>162</v>
       </c>
       <c r="BI41" t="s">
         <v>162</v>
@@ -10521,19 +10657,19 @@
         <v>162</v>
       </c>
       <c r="BK41" s="3" t="s">
-        <v>533</v>
+        <v>162</v>
       </c>
       <c r="BL41" t="s">
         <v>162</v>
       </c>
       <c r="BM41" s="3" t="s">
-        <v>533</v>
+        <v>162</v>
       </c>
       <c r="BN41" t="s">
         <v>162</v>
       </c>
       <c r="BO41" s="3" t="s">
-        <v>533</v>
+        <v>162</v>
       </c>
       <c r="BP41" t="s">
         <v>162</v>
@@ -10610,46 +10746,46 @@
         <v>163</v>
       </c>
       <c r="D42" t="s">
-        <v>530</v>
+        <v>528</v>
       </c>
       <c r="E42" t="s">
-        <v>530</v>
+        <v>528</v>
       </c>
       <c r="F42" s="3" t="s">
-        <v>389</v>
+        <v>282</v>
       </c>
       <c r="G42" s="3" t="s">
-        <v>389</v>
+        <v>282</v>
       </c>
       <c r="H42" t="s">
         <v>163</v>
       </c>
       <c r="I42" s="3" t="s">
-        <v>389</v>
+        <v>282</v>
       </c>
       <c r="J42" s="3" t="s">
-        <v>533</v>
+        <v>162</v>
       </c>
       <c r="K42" s="3" t="s">
-        <v>389</v>
+        <v>282</v>
       </c>
       <c r="L42" s="3" t="s">
-        <v>389</v>
+        <v>282</v>
       </c>
       <c r="M42" t="s">
         <v>163</v>
       </c>
       <c r="N42" t="s">
-        <v>530</v>
+        <v>528</v>
       </c>
       <c r="O42" t="s">
         <v>163</v>
       </c>
       <c r="P42" s="3" t="s">
-        <v>533</v>
+        <v>162</v>
       </c>
       <c r="Q42" t="s">
-        <v>530</v>
+        <v>528</v>
       </c>
       <c r="R42" t="s">
         <v>163</v>
@@ -10661,19 +10797,19 @@
         <v>163</v>
       </c>
       <c r="U42" t="s">
-        <v>389</v>
+        <v>282</v>
       </c>
       <c r="V42" s="58" t="s">
-        <v>531</v>
+        <v>529</v>
       </c>
       <c r="W42" t="s">
         <v>162</v>
       </c>
       <c r="X42" s="3" t="s">
-        <v>389</v>
+        <v>282</v>
       </c>
       <c r="Y42" s="3" t="s">
-        <v>389</v>
+        <v>282</v>
       </c>
       <c r="Z42" t="s">
         <v>163</v>
@@ -10688,10 +10824,10 @@
         <v>162</v>
       </c>
       <c r="AD42" s="3" t="s">
-        <v>389</v>
+        <v>282</v>
       </c>
       <c r="AE42" t="s">
-        <v>530</v>
+        <v>528</v>
       </c>
       <c r="AF42" t="s">
         <v>163</v>
@@ -10700,13 +10836,13 @@
         <v>163</v>
       </c>
       <c r="AH42" s="3" t="s">
-        <v>533</v>
+        <v>162</v>
       </c>
       <c r="AI42" t="s">
         <v>163</v>
       </c>
       <c r="AJ42" t="s">
-        <v>530</v>
+        <v>528</v>
       </c>
       <c r="AK42" t="s">
         <v>282</v>
@@ -10715,7 +10851,7 @@
         <v>163</v>
       </c>
       <c r="AM42" t="s">
-        <v>530</v>
+        <v>528</v>
       </c>
       <c r="AN42" s="58" t="s">
         <v>163</v>
@@ -10724,10 +10860,10 @@
         <v>163</v>
       </c>
       <c r="AP42" t="s">
-        <v>530</v>
+        <v>528</v>
       </c>
       <c r="AQ42" t="s">
-        <v>389</v>
+        <v>282</v>
       </c>
       <c r="AR42" t="s">
         <v>163</v>
@@ -10736,40 +10872,40 @@
         <v>163</v>
       </c>
       <c r="AT42" t="s">
-        <v>530</v>
+        <v>528</v>
       </c>
       <c r="AU42" t="s">
-        <v>530</v>
+        <v>528</v>
       </c>
       <c r="AV42" t="s">
         <v>163</v>
       </c>
       <c r="AW42" s="58" t="s">
-        <v>531</v>
+        <v>529</v>
       </c>
       <c r="AX42" t="s">
         <v>163</v>
       </c>
       <c r="AY42" t="s">
-        <v>530</v>
+        <v>528</v>
       </c>
       <c r="AZ42" s="3" t="s">
-        <v>533</v>
+        <v>162</v>
       </c>
       <c r="BA42" t="s">
-        <v>530</v>
+        <v>528</v>
       </c>
       <c r="BB42" t="s">
         <v>162</v>
       </c>
       <c r="BC42" s="58" t="s">
-        <v>531</v>
+        <v>529</v>
       </c>
       <c r="BD42" t="s">
         <v>163</v>
       </c>
       <c r="BE42" s="58" t="s">
-        <v>531</v>
+        <v>529</v>
       </c>
       <c r="BF42" t="s">
         <v>163</v>
@@ -10778,22 +10914,22 @@
         <v>163</v>
       </c>
       <c r="BH42" t="s">
-        <v>530</v>
+        <v>528</v>
       </c>
       <c r="BI42" s="58" t="s">
         <v>163</v>
       </c>
       <c r="BJ42" t="s">
-        <v>530</v>
+        <v>528</v>
       </c>
       <c r="BK42" s="58" t="s">
-        <v>531</v>
+        <v>529</v>
       </c>
       <c r="BL42" t="s">
         <v>163</v>
       </c>
       <c r="BM42" t="s">
-        <v>530</v>
+        <v>528</v>
       </c>
       <c r="BN42" t="s">
         <v>163</v>
@@ -10876,34 +11012,34 @@
         <v>162</v>
       </c>
       <c r="D43" s="3" t="s">
-        <v>533</v>
+        <v>162</v>
       </c>
       <c r="E43" s="3" t="s">
-        <v>533</v>
+        <v>162</v>
       </c>
       <c r="F43" s="3" t="s">
-        <v>389</v>
+        <v>282</v>
       </c>
       <c r="G43" s="3" t="s">
-        <v>389</v>
+        <v>282</v>
       </c>
       <c r="H43" t="s">
         <v>163</v>
       </c>
       <c r="I43" s="3" t="s">
-        <v>389</v>
+        <v>282</v>
       </c>
       <c r="J43" t="s">
         <v>162</v>
       </c>
       <c r="K43" s="3" t="s">
-        <v>389</v>
+        <v>282</v>
       </c>
       <c r="L43" s="3" t="s">
-        <v>389</v>
+        <v>282</v>
       </c>
       <c r="M43" s="3" t="s">
-        <v>533</v>
+        <v>162</v>
       </c>
       <c r="N43" t="s">
         <v>162</v>
@@ -10912,7 +11048,7 @@
         <v>162</v>
       </c>
       <c r="P43" s="3" t="s">
-        <v>533</v>
+        <v>162</v>
       </c>
       <c r="Q43" t="s">
         <v>163</v>
@@ -10927,19 +11063,19 @@
         <v>162</v>
       </c>
       <c r="U43" t="s">
-        <v>389</v>
+        <v>282</v>
       </c>
       <c r="V43" t="s">
-        <v>530</v>
+        <v>528</v>
       </c>
       <c r="W43" s="3" t="s">
-        <v>533</v>
+        <v>162</v>
       </c>
       <c r="X43" s="3" t="s">
-        <v>389</v>
+        <v>282</v>
       </c>
       <c r="Y43" s="3" t="s">
-        <v>389</v>
+        <v>282</v>
       </c>
       <c r="Z43" t="s">
         <v>163</v>
@@ -10951,10 +11087,10 @@
         <v>162</v>
       </c>
       <c r="AC43" s="3" t="s">
-        <v>533</v>
+        <v>162</v>
       </c>
       <c r="AD43" s="3" t="s">
-        <v>389</v>
+        <v>282</v>
       </c>
       <c r="AE43" t="s">
         <v>163</v>
@@ -10963,67 +11099,67 @@
         <v>163</v>
       </c>
       <c r="AG43" s="58" t="s">
-        <v>531</v>
+        <v>529</v>
       </c>
       <c r="AH43" t="s">
         <v>163</v>
       </c>
       <c r="AI43" s="3" t="s">
-        <v>533</v>
+        <v>162</v>
       </c>
       <c r="AJ43" t="s">
         <v>163</v>
       </c>
       <c r="AK43" s="3" t="s">
-        <v>533</v>
+        <v>162</v>
       </c>
       <c r="AL43" s="3" t="s">
-        <v>533</v>
+        <v>162</v>
       </c>
       <c r="AM43" s="3" t="s">
-        <v>533</v>
+        <v>162</v>
       </c>
       <c r="AN43" t="s">
         <v>162</v>
       </c>
       <c r="AO43" s="3" t="s">
-        <v>533</v>
+        <v>162</v>
       </c>
       <c r="AP43" t="s">
         <v>162</v>
       </c>
       <c r="AQ43" t="s">
-        <v>389</v>
+        <v>282</v>
       </c>
       <c r="AR43" t="s">
         <v>163</v>
       </c>
       <c r="AS43" t="s">
-        <v>532</v>
+        <v>530</v>
       </c>
       <c r="AT43" s="3" t="s">
-        <v>533</v>
+        <v>162</v>
       </c>
       <c r="AU43" s="3" t="s">
-        <v>533</v>
+        <v>162</v>
       </c>
       <c r="AV43" t="s">
         <v>162</v>
       </c>
       <c r="AW43" t="s">
-        <v>532</v>
+        <v>530</v>
       </c>
       <c r="AX43" s="3" t="s">
-        <v>533</v>
+        <v>162</v>
       </c>
       <c r="AY43" s="3" t="s">
-        <v>533</v>
+        <v>162</v>
       </c>
       <c r="AZ43" t="s">
         <v>163</v>
       </c>
       <c r="BA43" s="3" t="s">
-        <v>533</v>
+        <v>162</v>
       </c>
       <c r="BB43" t="s">
         <v>162</v>
@@ -11032,7 +11168,7 @@
         <v>162</v>
       </c>
       <c r="BD43" t="s">
-        <v>533</v>
+        <v>162</v>
       </c>
       <c r="BE43" t="s">
         <v>162</v>
@@ -11044,22 +11180,22 @@
         <v>163</v>
       </c>
       <c r="BH43" s="3" t="s">
-        <v>533</v>
+        <v>162</v>
       </c>
       <c r="BI43" t="s">
         <v>162</v>
       </c>
       <c r="BJ43" t="s">
-        <v>532</v>
+        <v>530</v>
       </c>
       <c r="BK43" s="3" t="s">
-        <v>533</v>
+        <v>162</v>
       </c>
       <c r="BL43" t="s">
         <v>162</v>
       </c>
       <c r="BM43" s="3" t="s">
-        <v>533</v>
+        <v>162</v>
       </c>
       <c r="BN43" t="s">
         <v>162</v>
@@ -11136,37 +11272,37 @@
         <v>192</v>
       </c>
       <c r="B44" t="s">
-        <v>530</v>
+        <v>528</v>
       </c>
       <c r="C44" t="s">
-        <v>530</v>
+        <v>528</v>
       </c>
       <c r="D44" t="s">
         <v>162</v>
       </c>
       <c r="E44" s="3" t="s">
-        <v>533</v>
+        <v>162</v>
       </c>
       <c r="F44" s="3" t="s">
-        <v>389</v>
+        <v>282</v>
       </c>
       <c r="G44" s="3" t="s">
-        <v>389</v>
+        <v>282</v>
       </c>
       <c r="H44" t="s">
         <v>163</v>
       </c>
       <c r="I44" s="3" t="s">
-        <v>389</v>
+        <v>282</v>
       </c>
       <c r="J44" t="s">
         <v>162</v>
       </c>
       <c r="K44" s="3" t="s">
-        <v>389</v>
+        <v>282</v>
       </c>
       <c r="L44" s="3" t="s">
-        <v>389</v>
+        <v>282</v>
       </c>
       <c r="M44" t="s">
         <v>163</v>
@@ -11178,7 +11314,7 @@
         <v>162</v>
       </c>
       <c r="P44" s="3" t="s">
-        <v>533</v>
+        <v>162</v>
       </c>
       <c r="Q44" t="s">
         <v>163</v>
@@ -11190,22 +11326,22 @@
         <v>162</v>
       </c>
       <c r="T44" s="58" t="s">
-        <v>531</v>
+        <v>529</v>
       </c>
       <c r="U44" t="s">
-        <v>389</v>
+        <v>282</v>
       </c>
       <c r="V44" t="s">
-        <v>530</v>
+        <v>528</v>
       </c>
       <c r="W44" t="s">
         <v>162</v>
       </c>
       <c r="X44" s="3" t="s">
-        <v>389</v>
+        <v>282</v>
       </c>
       <c r="Y44" s="3" t="s">
-        <v>389</v>
+        <v>282</v>
       </c>
       <c r="Z44" t="s">
         <v>162</v>
@@ -11217,10 +11353,10 @@
         <v>162</v>
       </c>
       <c r="AC44" s="3" t="s">
-        <v>533</v>
+        <v>162</v>
       </c>
       <c r="AD44" s="3" t="s">
-        <v>389</v>
+        <v>282</v>
       </c>
       <c r="AE44" t="s">
         <v>163</v>
@@ -11232,40 +11368,40 @@
         <v>163</v>
       </c>
       <c r="AH44" s="3" t="s">
-        <v>533</v>
+        <v>162</v>
       </c>
       <c r="AI44" t="s">
+        <v>528</v>
+      </c>
+      <c r="AJ44" t="s">
+        <v>528</v>
+      </c>
+      <c r="AK44" s="3" t="s">
+        <v>162</v>
+      </c>
+      <c r="AL44" t="s">
         <v>530</v>
       </c>
-      <c r="AJ44" t="s">
+      <c r="AM44" t="s">
         <v>530</v>
       </c>
-      <c r="AK44" s="3" t="s">
-        <v>533</v>
-      </c>
-      <c r="AL44" t="s">
-        <v>532</v>
-      </c>
-      <c r="AM44" t="s">
-        <v>532</v>
-      </c>
       <c r="AN44" s="58" t="s">
-        <v>389</v>
+        <v>282</v>
       </c>
       <c r="AO44" t="s">
         <v>163</v>
       </c>
       <c r="AP44" t="s">
+        <v>528</v>
+      </c>
+      <c r="AQ44" t="s">
+        <v>282</v>
+      </c>
+      <c r="AR44" t="s">
         <v>530</v>
       </c>
-      <c r="AQ44" t="s">
-        <v>389</v>
-      </c>
-      <c r="AR44" t="s">
-        <v>532</v>
-      </c>
       <c r="AS44" t="s">
-        <v>532</v>
+        <v>530</v>
       </c>
       <c r="AT44" t="s">
         <v>163</v>
@@ -11280,16 +11416,16 @@
         <v>163</v>
       </c>
       <c r="AX44" s="3" t="s">
-        <v>533</v>
+        <v>162</v>
       </c>
       <c r="AY44" s="58" t="s">
-        <v>531</v>
+        <v>529</v>
       </c>
       <c r="AZ44" t="s">
-        <v>532</v>
+        <v>530</v>
       </c>
       <c r="BA44" t="s">
-        <v>532</v>
+        <v>530</v>
       </c>
       <c r="BB44" t="s">
         <v>162</v>
@@ -11298,7 +11434,7 @@
         <v>162</v>
       </c>
       <c r="BD44" s="58" t="s">
-        <v>531</v>
+        <v>529</v>
       </c>
       <c r="BE44" t="s">
         <v>162</v>
@@ -11310,13 +11446,13 @@
         <v>163</v>
       </c>
       <c r="BH44" s="3" t="s">
-        <v>533</v>
+        <v>162</v>
       </c>
       <c r="BI44" t="s">
         <v>163</v>
       </c>
       <c r="BJ44" s="58" t="s">
-        <v>531</v>
+        <v>529</v>
       </c>
       <c r="BK44" t="s">
         <v>162</v>
@@ -11325,13 +11461,13 @@
         <v>163</v>
       </c>
       <c r="BM44" s="3" t="s">
-        <v>533</v>
+        <v>162</v>
       </c>
       <c r="BN44" t="s">
         <v>162</v>
       </c>
       <c r="BO44" t="s">
-        <v>530</v>
+        <v>528</v>
       </c>
       <c r="BP44" t="s">
         <v>163</v>
@@ -11402,40 +11538,40 @@
         <v>193</v>
       </c>
       <c r="B45" t="s">
-        <v>530</v>
+        <v>528</v>
       </c>
       <c r="C45" t="s">
         <v>162</v>
       </c>
       <c r="D45" t="s">
-        <v>530</v>
+        <v>528</v>
       </c>
       <c r="E45" s="3" t="s">
-        <v>533</v>
+        <v>162</v>
       </c>
       <c r="F45" s="3" t="s">
-        <v>389</v>
+        <v>282</v>
       </c>
       <c r="G45" s="3" t="s">
-        <v>389</v>
+        <v>282</v>
       </c>
       <c r="H45" s="3" t="s">
-        <v>533</v>
+        <v>162</v>
       </c>
       <c r="I45" s="3" t="s">
-        <v>389</v>
+        <v>282</v>
       </c>
       <c r="J45" s="58" t="s">
-        <v>531</v>
+        <v>529</v>
       </c>
       <c r="K45" s="3" t="s">
-        <v>389</v>
+        <v>282</v>
       </c>
       <c r="L45" s="3" t="s">
-        <v>389</v>
+        <v>282</v>
       </c>
       <c r="M45" s="3" t="s">
-        <v>533</v>
+        <v>162</v>
       </c>
       <c r="N45" t="s">
         <v>162</v>
@@ -11444,7 +11580,7 @@
         <v>162</v>
       </c>
       <c r="P45" s="3" t="s">
-        <v>533</v>
+        <v>162</v>
       </c>
       <c r="Q45" t="s">
         <v>162</v>
@@ -11459,19 +11595,19 @@
         <v>162</v>
       </c>
       <c r="U45" t="s">
-        <v>389</v>
+        <v>282</v>
       </c>
       <c r="V45" t="s">
         <v>162</v>
       </c>
       <c r="W45" s="3" t="s">
-        <v>533</v>
+        <v>162</v>
       </c>
       <c r="X45" s="3" t="s">
-        <v>389</v>
+        <v>282</v>
       </c>
       <c r="Y45" s="3" t="s">
-        <v>389</v>
+        <v>282</v>
       </c>
       <c r="Z45" t="s">
         <v>162</v>
@@ -11480,34 +11616,34 @@
         <v>162</v>
       </c>
       <c r="AB45" t="s">
-        <v>530</v>
+        <v>528</v>
       </c>
       <c r="AC45" s="3" t="s">
-        <v>533</v>
+        <v>162</v>
       </c>
       <c r="AD45" s="3" t="s">
-        <v>389</v>
+        <v>282</v>
       </c>
       <c r="AE45" s="3" t="s">
-        <v>533</v>
+        <v>162</v>
       </c>
       <c r="AF45" t="s">
         <v>163</v>
       </c>
       <c r="AG45" s="58" t="s">
-        <v>531</v>
+        <v>529</v>
       </c>
       <c r="AH45" t="s">
-        <v>532</v>
+        <v>530</v>
       </c>
       <c r="AI45" s="3" t="s">
-        <v>533</v>
+        <v>162</v>
       </c>
       <c r="AJ45" t="s">
-        <v>530</v>
+        <v>528</v>
       </c>
       <c r="AK45" s="3" t="s">
-        <v>533</v>
+        <v>162</v>
       </c>
       <c r="AL45" t="s">
         <v>163</v>
@@ -11519,43 +11655,43 @@
         <v>162</v>
       </c>
       <c r="AO45" s="3" t="s">
-        <v>533</v>
+        <v>162</v>
       </c>
       <c r="AP45" t="s">
         <v>162</v>
       </c>
       <c r="AQ45" t="s">
-        <v>389</v>
+        <v>282</v>
       </c>
       <c r="AR45" t="s">
         <v>162</v>
       </c>
       <c r="AS45" t="s">
-        <v>532</v>
+        <v>530</v>
       </c>
       <c r="AT45" s="3" t="s">
-        <v>533</v>
+        <v>162</v>
       </c>
       <c r="AU45" s="3" t="s">
-        <v>533</v>
+        <v>162</v>
       </c>
       <c r="AV45" s="3" t="s">
-        <v>533</v>
+        <v>162</v>
       </c>
       <c r="AW45" t="s">
         <v>162</v>
       </c>
       <c r="AX45" s="3" t="s">
-        <v>533</v>
+        <v>162</v>
       </c>
       <c r="AY45" s="3" t="s">
-        <v>533</v>
+        <v>162</v>
       </c>
       <c r="AZ45" t="s">
         <v>163</v>
       </c>
       <c r="BA45" s="3" t="s">
-        <v>533</v>
+        <v>162</v>
       </c>
       <c r="BB45" t="s">
         <v>162</v>
@@ -11573,10 +11709,10 @@
         <v>162</v>
       </c>
       <c r="BG45" t="s">
-        <v>533</v>
+        <v>162</v>
       </c>
       <c r="BH45" s="3" t="s">
-        <v>533</v>
+        <v>162</v>
       </c>
       <c r="BI45" t="s">
         <v>162</v>
@@ -11591,7 +11727,7 @@
         <v>162</v>
       </c>
       <c r="BM45" s="3" t="s">
-        <v>533</v>
+        <v>162</v>
       </c>
       <c r="BN45" t="s">
         <v>163</v>
@@ -11666,18 +11802,18 @@
     <row r="46" spans="1:88" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
     <row r="48" spans="1:88" x14ac:dyDescent="0.15">
       <c r="A48" s="75" t="s">
-        <v>403</v>
+        <v>401</v>
       </c>
     </row>
   </sheetData>
   <dataConsolidate/>
-  <conditionalFormatting sqref="B13:C13 F13:G13 I13 K13:L13 N13:O13 AD13 AJ13 AQ13:AR13 BG13 BI13 BP13:BQ13 Q13:U13 X13:AB13">
+  <conditionalFormatting sqref="B13:C13 F13:G13 I13 K13:L13 N13:O13 Q13:U13 X13:AB13 AD13 AJ13 AQ13:AR13 BG13 BI13 BP13:BQ13">
     <cfRule type="containsText" dxfId="0" priority="5" operator="containsText" text="None">
       <formula>NOT(ISERROR(SEARCH("None",B13)))</formula>
     </cfRule>
   </conditionalFormatting>
   <dataValidations count="3">
-    <dataValidation type="decimal" operator="greaterThan" allowBlank="1" showDropDown="1" sqref="AR20:AS20 AR29:AS31 AR27:AS27 AR4:AS4 AX14:BA14 BS12:BT12 AU14:AV14 BV20:CJ20 AU6:AV12 BO14 AY11:BA12 BB14 BH14 AS14 BM14 BM6:BM12 BK14 BP6:BQ14 BO6:BO12 AY6:BB9 AR6:AR14 AS6:AS12 BF14 BJ14 BK6:BK12 BL14 AT10 BH11:BH12 BV4:CJ14 BV27:CJ31 AW14 AY29:BQ31 BD14 AY27:BQ27 AY4:BQ4 BE6:BH9 AU4:AW4 AU27:AW27 AU20:BQ20 AU29:AW31 AW6:AW9 AX6:AX12 AW11:AW12 BB11:BB12 BC14 BC6:BC12 BD6:BD12 BE14 BE10:BE12 BG10:BG14 BF10:BF12 BI6:BI14 BJ6:BJ12 BL6:BL12 BN6:BN12 BN14" xr:uid="{867E023D-9480-D642-8D7B-D9C030E60E5B}">
+    <dataValidation type="decimal" operator="greaterThan" allowBlank="1" showDropDown="1" sqref="AR20:AS20 AR29:AS31 AR27:AS27 AR4:AS4 BS12:BT12 BV20:CJ20 AU6:AV12 BH14 AS14 BP6:BQ14 AY6:BB9 AR6:AR14 AS6:AS12 AT10 BH11:BH12 BV4:CJ14 BV27:CJ31 AY29:BQ31 AY27:BQ27 AY4:BQ4 BE6:BH9 AU4:AW4 AU27:AW27 AU20:BQ20 AU29:AW31 AW6:AW9 AX6:AX12 AW11:AW12 AY11:BB12 BC6:BD12 AU14:BF14 BG10:BG14 BE10:BF12 BI6:BI14 BJ6:BO12 BJ14:BO14" xr:uid="{867E023D-9480-D642-8D7B-D9C030E60E5B}">
       <formula1>1</formula1>
     </dataValidation>
     <dataValidation type="custom" allowBlank="1" showDropDown="1" sqref="AT20 AT29:AT31 AT27 AT14" xr:uid="{0FADE96E-D3E8-7A49-9B89-7D5551E86AFD}">
@@ -11914,7 +12050,7 @@
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A19" s="58" t="s">
-        <v>402</v>
+        <v>400</v>
       </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.15">
@@ -12065,7 +12201,7 @@
     </row>
     <row r="46" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A46" s="58" t="s">
-        <v>404</v>
+        <v>402</v>
       </c>
       <c r="D46" s="58"/>
     </row>
@@ -12217,7 +12353,7 @@
     </row>
     <row r="72" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A72" s="58" t="s">
-        <v>401</v>
+        <v>399</v>
       </c>
     </row>
     <row r="73" spans="1:4" x14ac:dyDescent="0.15">
@@ -12393,7 +12529,7 @@
     </row>
     <row r="104" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A104" s="50" t="s">
-        <v>405</v>
+        <v>403</v>
       </c>
       <c r="D104" s="58"/>
     </row>
@@ -12439,13 +12575,13 @@
     </row>
     <row r="113" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A113" s="38" t="s">
-        <v>410</v>
+        <v>408</v>
       </c>
       <c r="D113" s="60"/>
     </row>
     <row r="114" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A114" s="38" t="s">
-        <v>409</v>
+        <v>407</v>
       </c>
       <c r="D114" s="58"/>
     </row>
@@ -12454,30 +12590,30 @@
     </row>
     <row r="117" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A117" s="50" t="s">
-        <v>523</v>
+        <v>521</v>
       </c>
     </row>
     <row r="118" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A118" s="58" t="s">
-        <v>524</v>
+        <v>522</v>
       </c>
       <c r="D118" s="15"/>
     </row>
     <row r="119" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A119" s="58" t="s">
-        <v>508</v>
+        <v>506</v>
       </c>
       <c r="D119" s="15"/>
     </row>
     <row r="120" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A120" s="50" t="s">
-        <v>525</v>
+        <v>523</v>
       </c>
       <c r="D120" s="15"/>
     </row>
     <row r="121" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A121" s="58" t="s">
-        <v>404</v>
+        <v>402</v>
       </c>
       <c r="D121" s="15"/>
     </row>
@@ -12486,19 +12622,19 @@
     </row>
     <row r="123" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A123" s="50" t="s">
-        <v>523</v>
+        <v>521</v>
       </c>
       <c r="D123" s="15"/>
     </row>
     <row r="124" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A124" s="5" t="s">
-        <v>515</v>
+        <v>513</v>
       </c>
       <c r="D124" s="15"/>
     </row>
     <row r="125" spans="1:4" s="5" customFormat="1" x14ac:dyDescent="0.15">
       <c r="A125" s="50" t="s">
-        <v>525</v>
+        <v>523</v>
       </c>
       <c r="D125" s="91"/>
     </row>

</xml_diff>